<commit_message>
Module 3 - Topic 3
</commit_message>
<xml_diff>
--- a/OTJ Tracker Data Engineer L5.xlsx
+++ b/OTJ Tracker Data Engineer L5.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\laho2188\Documents\GitHub\Learning-Journal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF98CD0C-CAA9-47DC-9CCA-89EEDB3F4BB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF354459-59C3-4F4E-9287-6B2987E9AC59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="495" uniqueCount="361">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="505" uniqueCount="365">
   <si>
     <t xml:space="preserve">Apprenticeship Training Log </t>
   </si>
@@ -1144,21 +1144,12 @@
     <t>OTJT Log, Appendix</t>
   </si>
   <si>
-    <t>19.09.2024</t>
-  </si>
-  <si>
-    <t>24.09.2024</t>
-  </si>
-  <si>
     <t>Changing the data source of the CleaningLog Power BI reports from daily downloaded Excel files, to live data from Data Lakehouse</t>
   </si>
   <si>
     <t>Webinar</t>
   </si>
   <si>
-    <t>Weekly</t>
-  </si>
-  <si>
     <t>Shadowing my manager Jay about data quality on our data sources</t>
   </si>
   <si>
@@ -1174,15 +1165,9 @@
     <t>Managing Data Projects and Products</t>
   </si>
   <si>
-    <t>Core reading list - K28</t>
-  </si>
-  <si>
     <t>LinkedIn Learning: Data Engineering Fundations</t>
   </si>
   <si>
-    <t>Shadowing - K4, K5, K9, S26</t>
-  </si>
-  <si>
     <t>Shadowing - K2, K14, K17, K18, S7, S9, S13, B1, B2, B6</t>
   </si>
   <si>
@@ -1196,6 +1181,33 @@
   </si>
   <si>
     <t>Other - K28, B6</t>
+  </si>
+  <si>
+    <t>Monthly</t>
+  </si>
+  <si>
+    <t>Core reading list - K28, K29, S29</t>
+  </si>
+  <si>
+    <t>Shadowing - K4, K5, K9, S26, B1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reports - K1, K3, K6, K7, K9, K10, K11, K21, K25, K28, K30, S1, S3, S6, S11, S12, S13, S19, S23, S26, B1, B2, B3, B5, </t>
+  </si>
+  <si>
+    <t>Creating an general sample Power Bi report for all clients, replacing/ removing any sensitive data</t>
+  </si>
+  <si>
+    <t>Checking with my colleague Jay M, the systems/apps implemented in the company to centralise them and to find the best solutions</t>
+  </si>
+  <si>
+    <t>NDG Linux Unhatched: Course + Certification</t>
+  </si>
+  <si>
+    <t>Shadowing - K1, K3, K5, K6, K7, K9, K10, K11, K12, K13, K16, K17, K21, K22, K24, K25, K26, K28, K29, K30, S2, S3, S5, S8, S11, S12, S13, S14, S17, S22, S23, S24, S25, S26, S27, S28, S29, B1, B2, B3, B4, B5, B6</t>
+  </si>
+  <si>
+    <t>Research (internal wikis, etc.) - K28, K29, S14, S28, S29, B1, B6</t>
   </si>
 </sst>
 </file>
@@ -2579,9 +2591,6 @@
     <xf numFmtId="0" fontId="25" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2637,41 +2646,48 @@
     <xf numFmtId="164" fontId="33" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="71" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="57" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="71" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="13" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -2681,12 +2697,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -2727,6 +2737,60 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
@@ -2748,24 +2812,6 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -2777,40 +2823,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="71" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="57" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="71" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="13" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -3290,8 +3302,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AP312"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5:H19"/>
+    <sheetView tabSelected="1" topLeftCell="A45" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3301,7 +3313,7 @@
     <col min="3" max="3" width="24.28515625" customWidth="1"/>
     <col min="4" max="4" width="15" customWidth="1"/>
     <col min="5" max="5" width="10" customWidth="1"/>
-    <col min="6" max="6" width="20" customWidth="1"/>
+    <col min="6" max="6" width="20.28515625" customWidth="1"/>
     <col min="7" max="7" width="11.140625" customWidth="1"/>
     <col min="8" max="8" width="22" customWidth="1"/>
     <col min="14" max="14" width="4.28515625" customWidth="1"/>
@@ -3356,12 +3368,12 @@
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
-      <c r="J2" s="175"/>
-      <c r="K2" s="176"/>
-      <c r="L2" s="176"/>
-      <c r="M2" s="176"/>
-      <c r="N2" s="176"/>
-      <c r="O2" s="177"/>
+      <c r="J2" s="196"/>
+      <c r="K2" s="197"/>
+      <c r="L2" s="197"/>
+      <c r="M2" s="197"/>
+      <c r="N2" s="197"/>
+      <c r="O2" s="198"/>
       <c r="P2" s="36"/>
       <c r="Q2" s="36"/>
       <c r="R2" s="2"/>
@@ -3392,14 +3404,14 @@
     </row>
     <row r="3" spans="1:42" ht="220.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6"/>
-      <c r="B3" s="181" t="s">
+      <c r="B3" s="178" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="181"/>
-      <c r="D3" s="181"/>
-      <c r="E3" s="181"/>
-      <c r="F3" s="181"/>
-      <c r="G3" s="182"/>
+      <c r="C3" s="178"/>
+      <c r="D3" s="178"/>
+      <c r="E3" s="178"/>
+      <c r="F3" s="178"/>
+      <c r="G3" s="179"/>
       <c r="H3" s="1"/>
       <c r="I3" s="2"/>
       <c r="J3" s="52"/>
@@ -3499,12 +3511,12 @@
       </c>
       <c r="H5" s="195"/>
       <c r="I5" s="2"/>
-      <c r="J5" s="178"/>
-      <c r="K5" s="179"/>
-      <c r="L5" s="179"/>
-      <c r="M5" s="179"/>
-      <c r="N5" s="179"/>
-      <c r="O5" s="180"/>
+      <c r="J5" s="180"/>
+      <c r="K5" s="181"/>
+      <c r="L5" s="181"/>
+      <c r="M5" s="181"/>
+      <c r="N5" s="181"/>
+      <c r="O5" s="182"/>
       <c r="P5" s="2"/>
       <c r="Q5" s="2"/>
       <c r="R5" s="2"/>
@@ -3539,10 +3551,10 @@
         <v>9</v>
       </c>
       <c r="C6" s="55" t="s">
-        <v>346</v>
-      </c>
-      <c r="D6" s="55" t="s">
-        <v>343</v>
+        <v>344</v>
+      </c>
+      <c r="D6" s="175">
+        <v>45554</v>
       </c>
       <c r="E6" s="132">
         <v>4</v>
@@ -3595,9 +3607,11 @@
       <c r="B7" s="77" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="56"/>
-      <c r="D7" s="133" t="s">
+      <c r="C7" s="55" t="s">
         <v>344</v>
+      </c>
+      <c r="D7" s="176">
+        <v>45582</v>
       </c>
       <c r="E7" s="56">
         <v>12</v>
@@ -3650,8 +3664,12 @@
       <c r="B8" s="77" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="56"/>
-      <c r="D8" s="133"/>
+      <c r="C8" s="55" t="s">
+        <v>344</v>
+      </c>
+      <c r="D8" s="176">
+        <v>45617</v>
+      </c>
       <c r="E8" s="56">
         <v>15</v>
       </c>
@@ -3660,7 +3678,7 @@
       </c>
       <c r="G8" s="124">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="H8" s="195"/>
       <c r="I8" s="4"/>
@@ -4141,12 +4159,12 @@
       </c>
       <c r="H17" s="195"/>
       <c r="I17" s="4"/>
-      <c r="J17" s="178"/>
-      <c r="K17" s="179"/>
-      <c r="L17" s="179"/>
-      <c r="M17" s="179"/>
-      <c r="N17" s="179"/>
-      <c r="O17" s="180"/>
+      <c r="J17" s="180"/>
+      <c r="K17" s="181"/>
+      <c r="L17" s="181"/>
+      <c r="M17" s="181"/>
+      <c r="N17" s="181"/>
+      <c r="O17" s="182"/>
       <c r="P17" s="2"/>
       <c r="Q17" s="2"/>
       <c r="R17" s="2"/>
@@ -4245,7 +4263,7 @@
       </c>
       <c r="G19" s="128">
         <f>SUM(G6:G18)</f>
-        <v>31</v>
+        <v>63</v>
       </c>
       <c r="H19" s="195"/>
       <c r="I19" s="4"/>
@@ -4387,24 +4405,28 @@
       <c r="B22" s="56" t="s">
         <v>28</v>
       </c>
-      <c r="C22" s="56"/>
-      <c r="D22" s="56"/>
+      <c r="C22" s="133" t="s">
+        <v>24</v>
+      </c>
+      <c r="D22" s="177">
+        <v>45617</v>
+      </c>
       <c r="E22" s="56">
         <v>24</v>
       </c>
       <c r="F22" s="56"/>
       <c r="G22" s="56">
         <f>IF(NOT(ISBLANK(D22)), SUM(E22:F22), 0)</f>
-        <v>0</v>
-      </c>
-      <c r="H22" s="167"/>
+        <v>24</v>
+      </c>
+      <c r="H22" s="203"/>
       <c r="I22" s="2"/>
-      <c r="J22" s="178"/>
-      <c r="K22" s="179"/>
-      <c r="L22" s="179"/>
-      <c r="M22" s="179"/>
-      <c r="N22" s="179"/>
-      <c r="O22" s="180"/>
+      <c r="J22" s="180"/>
+      <c r="K22" s="181"/>
+      <c r="L22" s="181"/>
+      <c r="M22" s="181"/>
+      <c r="N22" s="181"/>
+      <c r="O22" s="182"/>
       <c r="P22" s="2"/>
       <c r="Q22" s="2"/>
       <c r="R22" s="2"/>
@@ -4448,7 +4470,7 @@
         <f>IF(NOT(ISBLANK(D23)), SUM(E23:F23), 0)</f>
         <v>0</v>
       </c>
-      <c r="H23" s="167"/>
+      <c r="H23" s="203"/>
       <c r="I23" s="2"/>
       <c r="J23" s="2"/>
       <c r="K23" s="2"/>
@@ -4499,7 +4521,7 @@
         <f>IF(NOT(ISBLANK(D24)), SUM(E24:F24), 0)</f>
         <v>0</v>
       </c>
-      <c r="H24" s="167"/>
+      <c r="H24" s="203"/>
       <c r="I24" s="2"/>
       <c r="J24" s="2"/>
       <c r="K24" s="2"/>
@@ -4550,7 +4572,7 @@
         <f>IF(NOT(ISBLANK(D25)), SUM(E25:F25), 0)</f>
         <v>0</v>
       </c>
-      <c r="H25" s="167"/>
+      <c r="H25" s="203"/>
       <c r="I25" s="2"/>
       <c r="J25" s="2"/>
       <c r="K25" s="2"/>
@@ -4601,7 +4623,7 @@
         <f>IF(NOT(ISBLANK(D26)), SUM(E26:F26), 0)</f>
         <v>0</v>
       </c>
-      <c r="H26" s="167"/>
+      <c r="H26" s="203"/>
       <c r="I26" s="2"/>
       <c r="J26" s="2"/>
       <c r="K26" s="2"/>
@@ -4645,7 +4667,7 @@
       <c r="E27" s="56"/>
       <c r="F27" s="56"/>
       <c r="G27" s="56"/>
-      <c r="H27" s="167"/>
+      <c r="H27" s="203"/>
       <c r="I27" s="2"/>
       <c r="J27" s="2"/>
       <c r="K27" s="2"/>
@@ -4698,9 +4720,9 @@
       </c>
       <c r="G28" s="58">
         <f>SUM(G22:H27)</f>
-        <v>0</v>
-      </c>
-      <c r="H28" s="167"/>
+        <v>24</v>
+      </c>
+      <c r="H28" s="203"/>
       <c r="I28" s="4"/>
       <c r="J28" s="2"/>
       <c r="K28" s="2"/>
@@ -4746,12 +4768,12 @@
       <c r="G29" s="190"/>
       <c r="H29" s="191"/>
       <c r="I29" s="2"/>
-      <c r="J29" s="178"/>
-      <c r="K29" s="179"/>
-      <c r="L29" s="179"/>
-      <c r="M29" s="179"/>
-      <c r="N29" s="179"/>
-      <c r="O29" s="180"/>
+      <c r="J29" s="180"/>
+      <c r="K29" s="181"/>
+      <c r="L29" s="181"/>
+      <c r="M29" s="181"/>
+      <c r="N29" s="181"/>
+      <c r="O29" s="182"/>
       <c r="P29" s="2"/>
       <c r="Q29" s="2"/>
       <c r="R29" s="2"/>
@@ -5011,23 +5033,23 @@
       <c r="D35" s="61" t="s">
         <v>38</v>
       </c>
-      <c r="E35" s="172" t="s">
+      <c r="E35" s="202" t="s">
         <v>39</v>
       </c>
-      <c r="F35" s="172"/>
+      <c r="F35" s="202"/>
       <c r="G35" s="61" t="s">
         <v>26</v>
       </c>
-      <c r="H35" s="168" t="s">
+      <c r="H35" s="204" t="s">
         <v>40</v>
       </c>
       <c r="I35" s="4"/>
-      <c r="J35" s="178"/>
-      <c r="K35" s="179"/>
-      <c r="L35" s="179"/>
-      <c r="M35" s="179"/>
-      <c r="N35" s="179"/>
-      <c r="O35" s="180"/>
+      <c r="J35" s="180"/>
+      <c r="K35" s="181"/>
+      <c r="L35" s="181"/>
+      <c r="M35" s="181"/>
+      <c r="N35" s="181"/>
+      <c r="O35" s="182"/>
       <c r="P35" s="2"/>
       <c r="Q35" s="2"/>
       <c r="R35" s="2"/>
@@ -5059,7 +5081,7 @@
     <row r="36" spans="1:42" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="60"/>
       <c r="B36" s="77" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="C36" s="142" t="s">
         <v>145</v>
@@ -5067,14 +5089,14 @@
       <c r="D36" s="143">
         <v>45559</v>
       </c>
-      <c r="E36" s="173" t="s">
-        <v>349</v>
-      </c>
-      <c r="F36" s="174"/>
+      <c r="E36" s="200" t="s">
+        <v>346</v>
+      </c>
+      <c r="F36" s="201"/>
       <c r="G36" s="145">
         <v>3</v>
       </c>
-      <c r="H36" s="169"/>
+      <c r="H36" s="205"/>
       <c r="I36" s="4"/>
       <c r="J36" s="2"/>
       <c r="K36" s="2"/>
@@ -5113,7 +5135,7 @@
     <row r="37" spans="1:42" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="60"/>
       <c r="B37" s="77" t="s">
-        <v>355</v>
+        <v>358</v>
       </c>
       <c r="C37" s="142" t="s">
         <v>146</v>
@@ -5121,14 +5143,14 @@
       <c r="D37" s="144">
         <v>45572</v>
       </c>
-      <c r="E37" s="173" t="s">
-        <v>348</v>
-      </c>
-      <c r="F37" s="174"/>
+      <c r="E37" s="200" t="s">
+        <v>345</v>
+      </c>
+      <c r="F37" s="201"/>
       <c r="G37" s="145">
         <v>4</v>
       </c>
-      <c r="H37" s="169"/>
+      <c r="H37" s="205"/>
       <c r="I37" s="5"/>
       <c r="J37" s="183"/>
       <c r="K37" s="184"/>
@@ -5167,7 +5189,7 @@
     <row r="38" spans="1:42" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="3"/>
       <c r="B38" s="77" t="s">
-        <v>353</v>
+        <v>357</v>
       </c>
       <c r="C38" s="142" t="s">
         <v>147</v>
@@ -5175,14 +5197,14 @@
       <c r="D38" s="143">
         <v>45575</v>
       </c>
-      <c r="E38" s="173" t="s">
-        <v>354</v>
-      </c>
-      <c r="F38" s="174"/>
+      <c r="E38" s="200" t="s">
+        <v>350</v>
+      </c>
+      <c r="F38" s="201"/>
       <c r="G38" s="145">
         <v>3</v>
       </c>
-      <c r="H38" s="169"/>
+      <c r="H38" s="205"/>
       <c r="I38" s="2"/>
       <c r="J38" s="2"/>
       <c r="K38" s="2"/>
@@ -5221,7 +5243,7 @@
     <row r="39" spans="1:42" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="3"/>
       <c r="B39" s="77" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="C39" s="142" t="s">
         <v>147</v>
@@ -5229,21 +5251,21 @@
       <c r="D39" s="143">
         <v>45579</v>
       </c>
-      <c r="E39" s="173" t="s">
-        <v>352</v>
-      </c>
-      <c r="F39" s="174"/>
+      <c r="E39" s="200" t="s">
+        <v>349</v>
+      </c>
+      <c r="F39" s="201"/>
       <c r="G39" s="145">
         <v>3</v>
       </c>
-      <c r="H39" s="169"/>
+      <c r="H39" s="205"/>
       <c r="I39" s="2"/>
-      <c r="J39" s="178"/>
-      <c r="K39" s="179"/>
-      <c r="L39" s="179"/>
-      <c r="M39" s="179"/>
-      <c r="N39" s="179"/>
-      <c r="O39" s="180"/>
+      <c r="J39" s="180"/>
+      <c r="K39" s="181"/>
+      <c r="L39" s="181"/>
+      <c r="M39" s="181"/>
+      <c r="N39" s="181"/>
+      <c r="O39" s="182"/>
       <c r="P39" s="2"/>
       <c r="Q39" s="2"/>
       <c r="R39" s="2"/>
@@ -5275,7 +5297,7 @@
     <row r="40" spans="1:42" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="3"/>
       <c r="B40" s="77" t="s">
-        <v>356</v>
+        <v>351</v>
       </c>
       <c r="C40" s="142" t="s">
         <v>149</v>
@@ -5283,14 +5305,14 @@
       <c r="D40" s="143">
         <v>45586</v>
       </c>
-      <c r="E40" s="173" t="s">
-        <v>345</v>
-      </c>
-      <c r="F40" s="174"/>
+      <c r="E40" s="200" t="s">
+        <v>343</v>
+      </c>
+      <c r="F40" s="201"/>
       <c r="G40" s="145">
         <v>8</v>
       </c>
-      <c r="H40" s="169"/>
+      <c r="H40" s="205"/>
       <c r="I40" s="2"/>
       <c r="J40" s="2"/>
       <c r="K40" s="2"/>
@@ -5329,22 +5351,22 @@
     <row r="41" spans="1:42" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="3"/>
       <c r="B41" s="77" t="s">
-        <v>357</v>
-      </c>
-      <c r="C41" s="156" t="s">
+        <v>352</v>
+      </c>
+      <c r="C41" s="155" t="s">
         <v>150</v>
       </c>
-      <c r="D41" s="224">
+      <c r="D41" s="174">
         <v>45597</v>
       </c>
-      <c r="E41" s="173" t="s">
-        <v>358</v>
-      </c>
-      <c r="F41" s="174"/>
+      <c r="E41" s="200" t="s">
+        <v>353</v>
+      </c>
+      <c r="F41" s="201"/>
       <c r="G41" s="145">
         <v>3</v>
       </c>
-      <c r="H41" s="169"/>
+      <c r="H41" s="205"/>
       <c r="I41" s="2"/>
       <c r="J41" s="2"/>
       <c r="K41" s="2"/>
@@ -5383,22 +5405,22 @@
     <row r="42" spans="1:42" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="3"/>
       <c r="B42" s="77" t="s">
-        <v>360</v>
-      </c>
-      <c r="C42" s="156" t="s">
+        <v>355</v>
+      </c>
+      <c r="C42" s="155" t="s">
         <v>151</v>
       </c>
-      <c r="D42" s="224">
+      <c r="D42" s="174">
         <v>45601</v>
       </c>
-      <c r="E42" s="173" t="s">
-        <v>359</v>
-      </c>
-      <c r="F42" s="174"/>
+      <c r="E42" s="200" t="s">
+        <v>354</v>
+      </c>
+      <c r="F42" s="201"/>
       <c r="G42" s="145">
         <v>2</v>
       </c>
-      <c r="H42" s="169"/>
+      <c r="H42" s="205"/>
       <c r="I42" s="2"/>
       <c r="J42" s="2"/>
       <c r="K42" s="2"/>
@@ -5434,15 +5456,25 @@
       <c r="AO42" s="2"/>
       <c r="AP42" s="2"/>
     </row>
-    <row r="43" spans="1:42" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:42" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="3"/>
-      <c r="B43" s="77"/>
-      <c r="C43" s="156"/>
-      <c r="D43" s="151"/>
-      <c r="E43" s="166"/>
-      <c r="F43" s="166"/>
-      <c r="G43" s="145"/>
-      <c r="H43" s="169"/>
+      <c r="B43" s="77" t="s">
+        <v>359</v>
+      </c>
+      <c r="C43" s="155" t="s">
+        <v>153</v>
+      </c>
+      <c r="D43" s="150">
+        <v>45609</v>
+      </c>
+      <c r="E43" s="200" t="s">
+        <v>360</v>
+      </c>
+      <c r="F43" s="201"/>
+      <c r="G43" s="145">
+        <v>8</v>
+      </c>
+      <c r="H43" s="205"/>
       <c r="I43" s="2"/>
       <c r="J43" s="2"/>
       <c r="K43" s="2"/>
@@ -5478,15 +5510,25 @@
       <c r="AO43" s="2"/>
       <c r="AP43" s="2"/>
     </row>
-    <row r="44" spans="1:42" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:42" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="3"/>
-      <c r="B44" s="77"/>
-      <c r="C44" s="156"/>
-      <c r="D44" s="151"/>
-      <c r="E44" s="166"/>
-      <c r="F44" s="166"/>
-      <c r="G44" s="146"/>
-      <c r="H44" s="169"/>
+      <c r="B44" s="77" t="s">
+        <v>363</v>
+      </c>
+      <c r="C44" s="155" t="s">
+        <v>156</v>
+      </c>
+      <c r="D44" s="150">
+        <v>45614</v>
+      </c>
+      <c r="E44" s="200" t="s">
+        <v>361</v>
+      </c>
+      <c r="F44" s="201"/>
+      <c r="G44" s="145">
+        <v>12</v>
+      </c>
+      <c r="H44" s="205"/>
       <c r="I44" s="2"/>
       <c r="J44" s="2"/>
       <c r="K44" s="2"/>
@@ -5522,15 +5564,25 @@
       <c r="AO44" s="2"/>
       <c r="AP44" s="2"/>
     </row>
-    <row r="45" spans="1:42" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:42" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="3"/>
-      <c r="B45" s="77"/>
-      <c r="C45" s="156"/>
-      <c r="D45" s="151"/>
-      <c r="E45" s="166"/>
-      <c r="F45" s="166"/>
-      <c r="G45" s="145"/>
-      <c r="H45" s="169"/>
+      <c r="B45" s="77" t="s">
+        <v>364</v>
+      </c>
+      <c r="C45" s="155" t="s">
+        <v>158</v>
+      </c>
+      <c r="D45" s="150">
+        <v>45623</v>
+      </c>
+      <c r="E45" s="200" t="s">
+        <v>362</v>
+      </c>
+      <c r="F45" s="201"/>
+      <c r="G45" s="145">
+        <v>5</v>
+      </c>
+      <c r="H45" s="205"/>
       <c r="I45" s="2"/>
       <c r="J45" s="2"/>
       <c r="K45" s="2"/>
@@ -5569,12 +5621,12 @@
     <row r="46" spans="1:42" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="3"/>
       <c r="B46" s="77"/>
-      <c r="C46" s="156"/>
-      <c r="D46" s="151"/>
-      <c r="E46" s="166"/>
-      <c r="F46" s="166"/>
+      <c r="C46" s="155"/>
+      <c r="D46" s="150"/>
+      <c r="E46" s="199"/>
+      <c r="F46" s="199"/>
       <c r="G46" s="145"/>
-      <c r="H46" s="169"/>
+      <c r="H46" s="205"/>
       <c r="I46" s="2"/>
       <c r="J46" s="2"/>
       <c r="K46" s="2"/>
@@ -5613,12 +5665,12 @@
     <row r="47" spans="1:42" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="3"/>
       <c r="B47" s="77"/>
-      <c r="C47" s="156"/>
-      <c r="D47" s="151"/>
-      <c r="E47" s="166"/>
-      <c r="F47" s="166"/>
+      <c r="C47" s="155"/>
+      <c r="D47" s="150"/>
+      <c r="E47" s="199"/>
+      <c r="F47" s="199"/>
       <c r="G47" s="145"/>
-      <c r="H47" s="169"/>
+      <c r="H47" s="205"/>
       <c r="I47" s="42"/>
       <c r="J47" s="36"/>
       <c r="K47" s="2"/>
@@ -5654,15 +5706,15 @@
       <c r="AO47" s="2"/>
       <c r="AP47" s="2"/>
     </row>
-    <row r="48" spans="1:42" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:42" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="3"/>
       <c r="B48" s="77"/>
       <c r="C48" s="142"/>
       <c r="D48" s="143"/>
-      <c r="E48" s="173"/>
-      <c r="F48" s="174"/>
+      <c r="E48" s="200"/>
+      <c r="F48" s="201"/>
       <c r="G48" s="145"/>
-      <c r="H48" s="169"/>
+      <c r="H48" s="205"/>
       <c r="I48" s="42"/>
       <c r="J48" s="36"/>
       <c r="K48" s="2"/>
@@ -5701,12 +5753,12 @@
     <row r="49" spans="1:42" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="3"/>
       <c r="B49" s="78"/>
-      <c r="C49" s="156"/>
-      <c r="D49" s="152"/>
-      <c r="E49" s="166"/>
-      <c r="F49" s="166"/>
-      <c r="G49" s="147"/>
-      <c r="H49" s="169"/>
+      <c r="C49" s="155"/>
+      <c r="D49" s="151"/>
+      <c r="E49" s="199"/>
+      <c r="F49" s="199"/>
+      <c r="G49" s="146"/>
+      <c r="H49" s="205"/>
       <c r="I49" s="2"/>
       <c r="J49" s="2"/>
       <c r="K49" s="2"/>
@@ -5745,12 +5797,12 @@
     <row r="50" spans="1:42" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="34"/>
       <c r="B50" s="75"/>
-      <c r="C50" s="156"/>
-      <c r="D50" s="152"/>
-      <c r="E50" s="166"/>
-      <c r="F50" s="166"/>
-      <c r="G50" s="147"/>
-      <c r="H50" s="169"/>
+      <c r="C50" s="155"/>
+      <c r="D50" s="151"/>
+      <c r="E50" s="199"/>
+      <c r="F50" s="199"/>
+      <c r="G50" s="146"/>
+      <c r="H50" s="205"/>
       <c r="I50" s="2"/>
       <c r="J50" s="2"/>
       <c r="K50" s="2"/>
@@ -5789,12 +5841,12 @@
     <row r="51" spans="1:42" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="3"/>
       <c r="B51" s="75"/>
-      <c r="C51" s="156"/>
-      <c r="D51" s="152"/>
-      <c r="E51" s="166"/>
-      <c r="F51" s="166"/>
-      <c r="G51" s="147"/>
-      <c r="H51" s="169"/>
+      <c r="C51" s="155"/>
+      <c r="D51" s="151"/>
+      <c r="E51" s="199"/>
+      <c r="F51" s="199"/>
+      <c r="G51" s="146"/>
+      <c r="H51" s="205"/>
       <c r="I51" s="2"/>
       <c r="J51" s="2"/>
       <c r="K51" s="2"/>
@@ -5833,12 +5885,12 @@
     <row r="52" spans="1:42" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="3"/>
       <c r="B52" s="75"/>
-      <c r="C52" s="156"/>
-      <c r="D52" s="152"/>
-      <c r="E52" s="166"/>
-      <c r="F52" s="166"/>
-      <c r="G52" s="147"/>
-      <c r="H52" s="169"/>
+      <c r="C52" s="155"/>
+      <c r="D52" s="151"/>
+      <c r="E52" s="199"/>
+      <c r="F52" s="199"/>
+      <c r="G52" s="146"/>
+      <c r="H52" s="205"/>
       <c r="I52" s="2"/>
       <c r="J52" s="2"/>
       <c r="K52" s="2"/>
@@ -5877,12 +5929,12 @@
     <row r="53" spans="1:42" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="3"/>
       <c r="B53" s="75"/>
-      <c r="C53" s="156"/>
-      <c r="D53" s="152"/>
-      <c r="E53" s="166"/>
-      <c r="F53" s="166"/>
-      <c r="G53" s="147"/>
-      <c r="H53" s="169"/>
+      <c r="C53" s="155"/>
+      <c r="D53" s="151"/>
+      <c r="E53" s="199"/>
+      <c r="F53" s="199"/>
+      <c r="G53" s="146"/>
+      <c r="H53" s="205"/>
       <c r="I53" s="2"/>
       <c r="J53" s="2"/>
       <c r="K53" s="2"/>
@@ -5921,12 +5973,12 @@
     <row r="54" spans="1:42" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="3"/>
       <c r="B54" s="75"/>
-      <c r="C54" s="156"/>
-      <c r="D54" s="152"/>
-      <c r="E54" s="166"/>
-      <c r="F54" s="166"/>
-      <c r="G54" s="147"/>
-      <c r="H54" s="169"/>
+      <c r="C54" s="155"/>
+      <c r="D54" s="151"/>
+      <c r="E54" s="199"/>
+      <c r="F54" s="199"/>
+      <c r="G54" s="146"/>
+      <c r="H54" s="205"/>
       <c r="I54" s="2"/>
       <c r="J54" s="2"/>
       <c r="K54" s="2"/>
@@ -5965,12 +6017,12 @@
     <row r="55" spans="1:42" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="3"/>
       <c r="B55" s="56"/>
-      <c r="C55" s="156"/>
-      <c r="D55" s="152"/>
-      <c r="E55" s="166"/>
-      <c r="F55" s="166"/>
-      <c r="G55" s="147"/>
-      <c r="H55" s="169"/>
+      <c r="C55" s="155"/>
+      <c r="D55" s="151"/>
+      <c r="E55" s="199"/>
+      <c r="F55" s="199"/>
+      <c r="G55" s="146"/>
+      <c r="H55" s="205"/>
       <c r="I55" s="2"/>
       <c r="J55" s="2"/>
       <c r="K55" s="2"/>
@@ -6009,12 +6061,12 @@
     <row r="56" spans="1:42" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="3"/>
       <c r="B56" s="56"/>
-      <c r="C56" s="156"/>
-      <c r="D56" s="152"/>
-      <c r="E56" s="166"/>
-      <c r="F56" s="166"/>
-      <c r="G56" s="147"/>
-      <c r="H56" s="169"/>
+      <c r="C56" s="155"/>
+      <c r="D56" s="151"/>
+      <c r="E56" s="199"/>
+      <c r="F56" s="199"/>
+      <c r="G56" s="146"/>
+      <c r="H56" s="205"/>
       <c r="I56" s="2"/>
       <c r="J56" s="2"/>
       <c r="K56" s="2"/>
@@ -6053,12 +6105,12 @@
     <row r="57" spans="1:42" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="3"/>
       <c r="B57" s="56"/>
-      <c r="C57" s="156"/>
-      <c r="D57" s="152"/>
-      <c r="E57" s="166"/>
-      <c r="F57" s="166"/>
-      <c r="G57" s="147"/>
-      <c r="H57" s="169"/>
+      <c r="C57" s="155"/>
+      <c r="D57" s="151"/>
+      <c r="E57" s="199"/>
+      <c r="F57" s="199"/>
+      <c r="G57" s="146"/>
+      <c r="H57" s="205"/>
       <c r="I57" s="2"/>
       <c r="J57" s="2"/>
       <c r="K57" s="2"/>
@@ -6097,12 +6149,12 @@
     <row r="58" spans="1:42" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="3"/>
       <c r="B58" s="56"/>
-      <c r="C58" s="156"/>
-      <c r="D58" s="152"/>
-      <c r="E58" s="166"/>
-      <c r="F58" s="166"/>
-      <c r="G58" s="147"/>
-      <c r="H58" s="169"/>
+      <c r="C58" s="155"/>
+      <c r="D58" s="151"/>
+      <c r="E58" s="199"/>
+      <c r="F58" s="199"/>
+      <c r="G58" s="146"/>
+      <c r="H58" s="205"/>
       <c r="I58" s="2"/>
       <c r="J58" s="2"/>
       <c r="K58" s="2"/>
@@ -6141,12 +6193,12 @@
     <row r="59" spans="1:42" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="3"/>
       <c r="B59" s="56"/>
-      <c r="C59" s="156"/>
-      <c r="D59" s="152"/>
-      <c r="E59" s="166"/>
-      <c r="F59" s="166"/>
-      <c r="G59" s="147"/>
-      <c r="H59" s="169"/>
+      <c r="C59" s="155"/>
+      <c r="D59" s="151"/>
+      <c r="E59" s="199"/>
+      <c r="F59" s="199"/>
+      <c r="G59" s="146"/>
+      <c r="H59" s="205"/>
       <c r="I59" s="2"/>
       <c r="J59" s="2"/>
       <c r="K59" s="2"/>
@@ -6185,12 +6237,12 @@
     <row r="60" spans="1:42" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="3"/>
       <c r="B60" s="56"/>
-      <c r="C60" s="156"/>
-      <c r="D60" s="152"/>
-      <c r="E60" s="166"/>
-      <c r="F60" s="166"/>
-      <c r="G60" s="147"/>
-      <c r="H60" s="169"/>
+      <c r="C60" s="155"/>
+      <c r="D60" s="151"/>
+      <c r="E60" s="199"/>
+      <c r="F60" s="199"/>
+      <c r="G60" s="146"/>
+      <c r="H60" s="205"/>
       <c r="I60" s="2"/>
       <c r="J60" s="2"/>
       <c r="K60" s="2"/>
@@ -6231,15 +6283,15 @@
       <c r="B61" s="121" t="s">
         <v>8</v>
       </c>
-      <c r="C61" s="157"/>
-      <c r="D61" s="153"/>
-      <c r="E61" s="171"/>
-      <c r="F61" s="171"/>
-      <c r="G61" s="148">
+      <c r="C61" s="156"/>
+      <c r="D61" s="152"/>
+      <c r="E61" s="207"/>
+      <c r="F61" s="207"/>
+      <c r="G61" s="147">
         <f>SUM(G36:G60)</f>
-        <v>26</v>
-      </c>
-      <c r="H61" s="170"/>
+        <v>51</v>
+      </c>
+      <c r="H61" s="206"/>
       <c r="I61" s="2"/>
       <c r="J61" s="2"/>
       <c r="K61" s="2"/>
@@ -6278,11 +6330,11 @@
     <row r="62" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A62" s="3"/>
       <c r="B62" s="123"/>
-      <c r="C62" s="158"/>
-      <c r="D62" s="154"/>
+      <c r="C62" s="157"/>
+      <c r="D62" s="153"/>
       <c r="E62" s="1"/>
       <c r="F62" s="1"/>
-      <c r="G62" s="149"/>
+      <c r="G62" s="148"/>
       <c r="H62" s="120"/>
       <c r="I62" s="2"/>
       <c r="J62" s="2"/>
@@ -6324,13 +6376,13 @@
       <c r="B63" s="122" t="s">
         <v>41</v>
       </c>
-      <c r="C63" s="159"/>
-      <c r="D63" s="155"/>
+      <c r="C63" s="158"/>
+      <c r="D63" s="154"/>
       <c r="E63" s="27"/>
       <c r="F63" s="27"/>
-      <c r="G63" s="150">
+      <c r="G63" s="149">
         <f>G61+G19+G28+G62</f>
-        <v>57</v>
+        <v>138</v>
       </c>
       <c r="H63" s="43"/>
       <c r="I63" s="2"/>
@@ -6416,7 +6468,6 @@
       <c r="A65" s="3"/>
       <c r="B65" s="1"/>
       <c r="D65" s="2"/>
-      <c r="E65" s="213"/>
       <c r="F65" s="2"/>
       <c r="G65" s="2"/>
       <c r="H65" s="36"/>
@@ -6465,7 +6516,6 @@
         <v>487</v>
       </c>
       <c r="D66" s="2"/>
-      <c r="E66" s="213"/>
       <c r="F66" s="2"/>
       <c r="G66" s="2"/>
       <c r="H66" s="36"/>
@@ -6511,10 +6561,9 @@
       </c>
       <c r="C67" s="56">
         <f>G63</f>
-        <v>57</v>
+        <v>138</v>
       </c>
       <c r="D67" s="2"/>
-      <c r="E67" s="213"/>
       <c r="F67" s="2"/>
       <c r="G67" s="2"/>
       <c r="H67" s="36"/>
@@ -6560,10 +6609,9 @@
       </c>
       <c r="C68" s="58">
         <f>C66-C67</f>
-        <v>430</v>
+        <v>349</v>
       </c>
       <c r="D68" s="2"/>
-      <c r="E68" s="213"/>
       <c r="F68" s="2"/>
       <c r="G68" s="2"/>
       <c r="H68" s="36"/>
@@ -6606,7 +6654,6 @@
       <c r="A69" s="3"/>
       <c r="B69" s="2"/>
       <c r="D69" s="2"/>
-      <c r="E69" s="213"/>
       <c r="F69" s="2"/>
       <c r="G69" s="2"/>
       <c r="H69" s="36"/>
@@ -6649,7 +6696,6 @@
       <c r="A70" s="3"/>
       <c r="B70" s="2"/>
       <c r="D70" s="2"/>
-      <c r="E70" s="213"/>
       <c r="F70" s="2"/>
       <c r="G70" s="2"/>
       <c r="H70" s="2"/>
@@ -6692,7 +6738,6 @@
       <c r="A71" s="3"/>
       <c r="B71" s="2"/>
       <c r="D71" s="2"/>
-      <c r="E71" s="213"/>
       <c r="F71" s="2"/>
       <c r="G71" s="2"/>
       <c r="H71" s="2"/>
@@ -12447,32 +12492,6 @@
     </row>
   </sheetData>
   <mergeCells count="42">
-    <mergeCell ref="B3:G3"/>
-    <mergeCell ref="J35:O35"/>
-    <mergeCell ref="J37:O37"/>
-    <mergeCell ref="J39:O39"/>
-    <mergeCell ref="J30:O30"/>
-    <mergeCell ref="B29:H29"/>
-    <mergeCell ref="B31:F31"/>
-    <mergeCell ref="H5:H19"/>
-    <mergeCell ref="J2:O2"/>
-    <mergeCell ref="J29:O29"/>
-    <mergeCell ref="J17:O17"/>
-    <mergeCell ref="J5:O5"/>
-    <mergeCell ref="J22:O22"/>
-    <mergeCell ref="E55:F55"/>
-    <mergeCell ref="E56:F56"/>
-    <mergeCell ref="E45:F45"/>
-    <mergeCell ref="E46:F46"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="E50:F50"/>
-    <mergeCell ref="E51:F51"/>
-    <mergeCell ref="E52:F52"/>
-    <mergeCell ref="E53:F53"/>
-    <mergeCell ref="E54:F54"/>
     <mergeCell ref="E57:F57"/>
     <mergeCell ref="H22:H28"/>
     <mergeCell ref="H35:H61"/>
@@ -12489,6 +12508,32 @@
     <mergeCell ref="E47:F47"/>
     <mergeCell ref="E48:F48"/>
     <mergeCell ref="E49:F49"/>
+    <mergeCell ref="E55:F55"/>
+    <mergeCell ref="E56:F56"/>
+    <mergeCell ref="E45:F45"/>
+    <mergeCell ref="E46:F46"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="E50:F50"/>
+    <mergeCell ref="E51:F51"/>
+    <mergeCell ref="E52:F52"/>
+    <mergeCell ref="E53:F53"/>
+    <mergeCell ref="E54:F54"/>
+    <mergeCell ref="J2:O2"/>
+    <mergeCell ref="J29:O29"/>
+    <mergeCell ref="J17:O17"/>
+    <mergeCell ref="J5:O5"/>
+    <mergeCell ref="J22:O22"/>
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="J35:O35"/>
+    <mergeCell ref="J37:O37"/>
+    <mergeCell ref="J39:O39"/>
+    <mergeCell ref="J30:O30"/>
+    <mergeCell ref="B29:H29"/>
+    <mergeCell ref="B31:F31"/>
+    <mergeCell ref="H5:H19"/>
   </mergeCells>
   <phoneticPr fontId="24" type="noConversion"/>
   <dataValidations count="6">
@@ -12508,7 +12553,7 @@
           <x14:formula1>
             <xm:f>'List - Hide'!$D$2:$D$3</xm:f>
           </x14:formula1>
-          <xm:sqref>C7:C20 C33</xm:sqref>
+          <xm:sqref>C33 C9:C20</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Entry!" error="Please pick from the list!" prompt="Please select from the list" xr:uid="{00000000-0002-0000-0000-000007000000}">
           <x14:formula1>
@@ -12711,8 +12756,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:BS319"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView topLeftCell="A18" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12732,57 +12777,57 @@
       <c r="A1" s="137" t="s">
         <v>262</v>
       </c>
-      <c r="B1" s="221" t="s">
+      <c r="B1" s="171" t="s">
         <v>263</v>
       </c>
-      <c r="C1" s="221" t="s">
+      <c r="C1" s="171" t="s">
         <v>65</v>
       </c>
       <c r="D1" s="141" t="s">
         <v>262</v>
       </c>
-      <c r="E1" s="214" t="s">
+      <c r="E1" s="165" t="s">
         <v>295</v>
       </c>
-      <c r="F1" s="215" t="s">
+      <c r="F1" s="166" t="s">
         <v>66</v>
       </c>
       <c r="G1" s="141" t="s">
         <v>262</v>
       </c>
-      <c r="H1" s="223" t="s">
+      <c r="H1" s="173" t="s">
         <v>325</v>
       </c>
-      <c r="I1" s="215" t="s">
+      <c r="I1" s="166" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="2" spans="1:59" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="139" t="s">
-        <v>56</v>
-      </c>
-      <c r="B2" s="222" t="s">
+        <v>61</v>
+      </c>
+      <c r="B2" s="172" t="s">
         <v>264</v>
       </c>
-      <c r="C2" s="218" t="s">
+      <c r="C2" s="168" t="s">
         <v>68</v>
       </c>
-      <c r="D2" s="219" t="s">
+      <c r="D2" s="169" t="s">
         <v>61</v>
       </c>
-      <c r="E2" s="216" t="s">
+      <c r="E2" s="167" t="s">
         <v>294</v>
       </c>
-      <c r="F2" s="217" t="s">
+      <c r="F2" s="168" t="s">
         <v>69</v>
       </c>
-      <c r="G2" s="219" t="s">
-        <v>56</v>
-      </c>
-      <c r="H2" s="222" t="s">
+      <c r="G2" s="169" t="s">
+        <v>61</v>
+      </c>
+      <c r="H2" s="172" t="s">
         <v>324</v>
       </c>
-      <c r="I2" s="218" t="s">
+      <c r="I2" s="168" t="s">
         <v>70</v>
       </c>
       <c r="J2" s="135"/>
@@ -12840,28 +12885,28 @@
       <c r="A3" s="139" t="s">
         <v>61</v>
       </c>
-      <c r="B3" s="222" t="s">
+      <c r="B3" s="172" t="s">
         <v>265</v>
       </c>
-      <c r="C3" s="218" t="s">
+      <c r="C3" s="168" t="s">
         <v>71</v>
       </c>
-      <c r="D3" s="219" t="s">
-        <v>56</v>
-      </c>
-      <c r="E3" s="216" t="s">
+      <c r="D3" s="169" t="s">
+        <v>61</v>
+      </c>
+      <c r="E3" s="167" t="s">
         <v>296</v>
       </c>
-      <c r="F3" s="218" t="s">
+      <c r="F3" s="168" t="s">
         <v>72</v>
       </c>
-      <c r="G3" s="219" t="s">
-        <v>56</v>
-      </c>
-      <c r="H3" s="222" t="s">
+      <c r="G3" s="169" t="s">
+        <v>61</v>
+      </c>
+      <c r="H3" s="172" t="s">
         <v>326</v>
       </c>
-      <c r="I3" s="218" t="s">
+      <c r="I3" s="168" t="s">
         <v>73</v>
       </c>
       <c r="J3" s="135"/>
@@ -12917,30 +12962,30 @@
     </row>
     <row r="4" spans="1:59" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="139" t="s">
-        <v>56</v>
-      </c>
-      <c r="B4" s="222" t="s">
+        <v>61</v>
+      </c>
+      <c r="B4" s="172" t="s">
         <v>266</v>
       </c>
-      <c r="C4" s="218" t="s">
+      <c r="C4" s="168" t="s">
         <v>74</v>
       </c>
-      <c r="D4" s="219" t="s">
-        <v>56</v>
-      </c>
-      <c r="E4" s="216" t="s">
+      <c r="D4" s="169" t="s">
+        <v>61</v>
+      </c>
+      <c r="E4" s="167" t="s">
         <v>297</v>
       </c>
-      <c r="F4" s="218" t="s">
+      <c r="F4" s="168" t="s">
         <v>75</v>
       </c>
-      <c r="G4" s="219" t="s">
-        <v>56</v>
-      </c>
-      <c r="H4" s="222" t="s">
+      <c r="G4" s="169" t="s">
+        <v>61</v>
+      </c>
+      <c r="H4" s="172" t="s">
         <v>327</v>
       </c>
-      <c r="I4" s="218" t="s">
+      <c r="I4" s="168" t="s">
         <v>76</v>
       </c>
       <c r="J4" s="135"/>
@@ -12998,28 +13043,28 @@
       <c r="A5" s="139" t="s">
         <v>56</v>
       </c>
-      <c r="B5" s="222" t="s">
+      <c r="B5" s="172" t="s">
         <v>267</v>
       </c>
-      <c r="C5" s="218" t="s">
+      <c r="C5" s="168" t="s">
         <v>77</v>
       </c>
-      <c r="D5" s="219" t="s">
+      <c r="D5" s="169" t="s">
         <v>56</v>
       </c>
-      <c r="E5" s="216" t="s">
+      <c r="E5" s="167" t="s">
         <v>298</v>
       </c>
-      <c r="F5" s="218" t="s">
+      <c r="F5" s="168" t="s">
         <v>78</v>
       </c>
-      <c r="G5" s="219" t="s">
-        <v>56</v>
-      </c>
-      <c r="H5" s="222" t="s">
+      <c r="G5" s="169" t="s">
+        <v>61</v>
+      </c>
+      <c r="H5" s="172" t="s">
         <v>328</v>
       </c>
-      <c r="I5" s="218" t="s">
+      <c r="I5" s="168" t="s">
         <v>79</v>
       </c>
       <c r="J5" s="135"/>
@@ -13075,30 +13120,30 @@
     </row>
     <row r="6" spans="1:59" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="139" t="s">
-        <v>56</v>
-      </c>
-      <c r="B6" s="222" t="s">
+        <v>61</v>
+      </c>
+      <c r="B6" s="172" t="s">
         <v>268</v>
       </c>
-      <c r="C6" s="218" t="s">
+      <c r="C6" s="168" t="s">
         <v>80</v>
       </c>
-      <c r="D6" s="219" t="s">
+      <c r="D6" s="169" t="s">
         <v>61</v>
       </c>
-      <c r="E6" s="216" t="s">
+      <c r="E6" s="167" t="s">
         <v>299</v>
       </c>
-      <c r="F6" s="218" t="s">
+      <c r="F6" s="168" t="s">
         <v>81</v>
       </c>
-      <c r="G6" s="219" t="s">
-        <v>56</v>
-      </c>
-      <c r="H6" s="222" t="s">
+      <c r="G6" s="169" t="s">
+        <v>61</v>
+      </c>
+      <c r="H6" s="172" t="s">
         <v>329</v>
       </c>
-      <c r="I6" s="218" t="s">
+      <c r="I6" s="168" t="s">
         <v>82</v>
       </c>
       <c r="J6" s="135"/>
@@ -13156,28 +13201,28 @@
       <c r="A7" s="139" t="s">
         <v>61</v>
       </c>
-      <c r="B7" s="222" t="s">
+      <c r="B7" s="172" t="s">
         <v>269</v>
       </c>
-      <c r="C7" s="218" t="s">
+      <c r="C7" s="168" t="s">
         <v>83</v>
       </c>
-      <c r="D7" s="219" t="s">
-        <v>56</v>
-      </c>
-      <c r="E7" s="216" t="s">
+      <c r="D7" s="169" t="s">
+        <v>61</v>
+      </c>
+      <c r="E7" s="167" t="s">
         <v>300</v>
       </c>
-      <c r="F7" s="218" t="s">
+      <c r="F7" s="168" t="s">
         <v>84</v>
       </c>
-      <c r="G7" s="220" t="s">
-        <v>56</v>
-      </c>
-      <c r="H7" s="222" t="s">
+      <c r="G7" s="170" t="s">
+        <v>61</v>
+      </c>
+      <c r="H7" s="172" t="s">
         <v>330</v>
       </c>
-      <c r="I7" s="218" t="s">
+      <c r="I7" s="168" t="s">
         <v>85</v>
       </c>
       <c r="J7" s="135"/>
@@ -13233,21 +13278,21 @@
     </row>
     <row r="8" spans="1:59" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="139" t="s">
-        <v>56</v>
-      </c>
-      <c r="B8" s="222" t="s">
+        <v>61</v>
+      </c>
+      <c r="B8" s="172" t="s">
         <v>270</v>
       </c>
-      <c r="C8" s="218" t="s">
+      <c r="C8" s="168" t="s">
         <v>86</v>
       </c>
-      <c r="D8" s="219" t="s">
-        <v>56</v>
-      </c>
-      <c r="E8" s="216" t="s">
+      <c r="D8" s="169" t="s">
+        <v>61</v>
+      </c>
+      <c r="E8" s="167" t="s">
         <v>301</v>
       </c>
-      <c r="F8" s="218" t="s">
+      <c r="F8" s="168" t="s">
         <v>87</v>
       </c>
       <c r="G8" s="81"/>
@@ -13308,19 +13353,19 @@
       <c r="A9" s="139" t="s">
         <v>56</v>
       </c>
-      <c r="B9" s="222" t="s">
+      <c r="B9" s="172" t="s">
         <v>271</v>
       </c>
-      <c r="C9" s="218" t="s">
+      <c r="C9" s="168" t="s">
         <v>88</v>
       </c>
-      <c r="D9" s="219" t="s">
-        <v>56</v>
-      </c>
-      <c r="E9" s="216" t="s">
+      <c r="D9" s="169" t="s">
+        <v>61</v>
+      </c>
+      <c r="E9" s="167" t="s">
         <v>302</v>
       </c>
-      <c r="F9" s="218" t="s">
+      <c r="F9" s="168" t="s">
         <v>89</v>
       </c>
       <c r="G9" s="81"/>
@@ -13381,19 +13426,19 @@
       <c r="A10" s="139" t="s">
         <v>61</v>
       </c>
-      <c r="B10" s="222" t="s">
+      <c r="B10" s="172" t="s">
         <v>272</v>
       </c>
-      <c r="C10" s="218" t="s">
+      <c r="C10" s="168" t="s">
         <v>90</v>
       </c>
-      <c r="D10" s="219" t="s">
-        <v>56</v>
-      </c>
-      <c r="E10" s="216" t="s">
+      <c r="D10" s="169" t="s">
+        <v>61</v>
+      </c>
+      <c r="E10" s="167" t="s">
         <v>303</v>
       </c>
-      <c r="F10" s="218" t="s">
+      <c r="F10" s="168" t="s">
         <v>91</v>
       </c>
       <c r="G10" s="81"/>
@@ -13452,21 +13497,21 @@
     </row>
     <row r="11" spans="1:59" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="139" t="s">
+        <v>61</v>
+      </c>
+      <c r="B11" s="172" t="s">
+        <v>273</v>
+      </c>
+      <c r="C11" s="168" t="s">
+        <v>92</v>
+      </c>
+      <c r="D11" s="169" t="s">
         <v>56</v>
       </c>
-      <c r="B11" s="222" t="s">
-        <v>273</v>
-      </c>
-      <c r="C11" s="218" t="s">
-        <v>92</v>
-      </c>
-      <c r="D11" s="219" t="s">
-        <v>56</v>
-      </c>
-      <c r="E11" s="216" t="s">
+      <c r="E11" s="167" t="s">
         <v>304</v>
       </c>
-      <c r="F11" s="218" t="s">
+      <c r="F11" s="168" t="s">
         <v>93</v>
       </c>
       <c r="G11" s="81"/>
@@ -13525,21 +13570,21 @@
     </row>
     <row r="12" spans="1:59" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="139" t="s">
-        <v>56</v>
-      </c>
-      <c r="B12" s="222" t="s">
+        <v>61</v>
+      </c>
+      <c r="B12" s="172" t="s">
         <v>274</v>
       </c>
-      <c r="C12" s="218" t="s">
+      <c r="C12" s="168" t="s">
         <v>94</v>
       </c>
-      <c r="D12" s="219" t="s">
-        <v>56</v>
-      </c>
-      <c r="E12" s="216" t="s">
+      <c r="D12" s="169" t="s">
+        <v>61</v>
+      </c>
+      <c r="E12" s="167" t="s">
         <v>305</v>
       </c>
-      <c r="F12" s="218" t="s">
+      <c r="F12" s="168" t="s">
         <v>95</v>
       </c>
       <c r="G12" s="81"/>
@@ -13598,21 +13643,21 @@
     </row>
     <row r="13" spans="1:59" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="139" t="s">
-        <v>56</v>
-      </c>
-      <c r="B13" s="222" t="s">
+        <v>61</v>
+      </c>
+      <c r="B13" s="172" t="s">
         <v>275</v>
       </c>
-      <c r="C13" s="218" t="s">
+      <c r="C13" s="168" t="s">
         <v>96</v>
       </c>
-      <c r="D13" s="219" t="s">
-        <v>56</v>
-      </c>
-      <c r="E13" s="216" t="s">
+      <c r="D13" s="169" t="s">
+        <v>61</v>
+      </c>
+      <c r="E13" s="167" t="s">
         <v>306</v>
       </c>
-      <c r="F13" s="218" t="s">
+      <c r="F13" s="168" t="s">
         <v>97</v>
       </c>
       <c r="G13" s="81"/>
@@ -13671,21 +13716,21 @@
     </row>
     <row r="14" spans="1:59" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="139" t="s">
-        <v>56</v>
-      </c>
-      <c r="B14" s="222" t="s">
+        <v>61</v>
+      </c>
+      <c r="B14" s="172" t="s">
         <v>276</v>
       </c>
-      <c r="C14" s="218" t="s">
+      <c r="C14" s="168" t="s">
         <v>98</v>
       </c>
-      <c r="D14" s="219" t="s">
-        <v>56</v>
-      </c>
-      <c r="E14" s="216" t="s">
+      <c r="D14" s="169" t="s">
+        <v>61</v>
+      </c>
+      <c r="E14" s="167" t="s">
         <v>307</v>
       </c>
-      <c r="F14" s="218" t="s">
+      <c r="F14" s="168" t="s">
         <v>99</v>
       </c>
       <c r="G14" s="81"/>
@@ -13742,23 +13787,23 @@
       <c r="BF14" s="42"/>
       <c r="BG14" s="42"/>
     </row>
-    <row r="15" spans="1:59" ht="45" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:59" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="139" t="s">
         <v>56</v>
       </c>
-      <c r="B15" s="222" t="s">
+      <c r="B15" s="172" t="s">
         <v>277</v>
       </c>
-      <c r="C15" s="218" t="s">
+      <c r="C15" s="168" t="s">
         <v>100</v>
       </c>
-      <c r="D15" s="219" t="s">
-        <v>56</v>
-      </c>
-      <c r="E15" s="216" t="s">
+      <c r="D15" s="169" t="s">
+        <v>61</v>
+      </c>
+      <c r="E15" s="167" t="s">
         <v>308</v>
       </c>
-      <c r="F15" s="218" t="s">
+      <c r="F15" s="168" t="s">
         <v>101</v>
       </c>
       <c r="G15" s="81"/>
@@ -13817,21 +13862,21 @@
     </row>
     <row r="16" spans="1:59" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="139" t="s">
+        <v>61</v>
+      </c>
+      <c r="B16" s="172" t="s">
+        <v>278</v>
+      </c>
+      <c r="C16" s="168" t="s">
+        <v>102</v>
+      </c>
+      <c r="D16" s="169" t="s">
         <v>56</v>
       </c>
-      <c r="B16" s="222" t="s">
-        <v>278</v>
-      </c>
-      <c r="C16" s="218" t="s">
-        <v>102</v>
-      </c>
-      <c r="D16" s="219" t="s">
-        <v>56</v>
-      </c>
-      <c r="E16" s="216" t="s">
+      <c r="E16" s="167" t="s">
         <v>309</v>
       </c>
-      <c r="F16" s="218" t="s">
+      <c r="F16" s="168" t="s">
         <v>103</v>
       </c>
       <c r="G16" s="81"/>
@@ -13888,23 +13933,23 @@
       <c r="BF16" s="42"/>
       <c r="BG16" s="42"/>
     </row>
-    <row r="17" spans="1:59" ht="60" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:59" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="139" t="s">
         <v>61</v>
       </c>
-      <c r="B17" s="222" t="s">
+      <c r="B17" s="172" t="s">
         <v>279</v>
       </c>
-      <c r="C17" s="218" t="s">
+      <c r="C17" s="168" t="s">
         <v>104</v>
       </c>
-      <c r="D17" s="219" t="s">
+      <c r="D17" s="169" t="s">
         <v>56</v>
       </c>
-      <c r="E17" s="216" t="s">
+      <c r="E17" s="167" t="s">
         <v>310</v>
       </c>
-      <c r="F17" s="218" t="s">
+      <c r="F17" s="168" t="s">
         <v>105</v>
       </c>
       <c r="G17" s="81"/>
@@ -13963,21 +14008,21 @@
     </row>
     <row r="18" spans="1:59" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="139" t="s">
-        <v>56</v>
-      </c>
-      <c r="B18" s="222" t="s">
+        <v>61</v>
+      </c>
+      <c r="B18" s="172" t="s">
         <v>280</v>
       </c>
-      <c r="C18" s="218" t="s">
+      <c r="C18" s="168" t="s">
         <v>106</v>
       </c>
-      <c r="D18" s="219" t="s">
-        <v>56</v>
-      </c>
-      <c r="E18" s="216" t="s">
+      <c r="D18" s="169" t="s">
+        <v>61</v>
+      </c>
+      <c r="E18" s="167" t="s">
         <v>311</v>
       </c>
-      <c r="F18" s="218" t="s">
+      <c r="F18" s="168" t="s">
         <v>107</v>
       </c>
       <c r="G18" s="81"/>
@@ -14038,19 +14083,19 @@
       <c r="A19" s="139" t="s">
         <v>61</v>
       </c>
-      <c r="B19" s="222" t="s">
+      <c r="B19" s="172" t="s">
         <v>281</v>
       </c>
-      <c r="C19" s="218" t="s">
+      <c r="C19" s="168" t="s">
         <v>108</v>
       </c>
-      <c r="D19" s="219" t="s">
+      <c r="D19" s="169" t="s">
         <v>56</v>
       </c>
-      <c r="E19" s="216" t="s">
+      <c r="E19" s="167" t="s">
         <v>312</v>
       </c>
-      <c r="F19" s="218" t="s">
+      <c r="F19" s="168" t="s">
         <v>109</v>
       </c>
       <c r="G19" s="81"/>
@@ -14109,21 +14154,21 @@
     </row>
     <row r="20" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A20" s="139" t="s">
-        <v>56</v>
-      </c>
-      <c r="B20" s="222" t="s">
+        <v>61</v>
+      </c>
+      <c r="B20" s="172" t="s">
         <v>282</v>
       </c>
-      <c r="C20" s="218" t="s">
+      <c r="C20" s="168" t="s">
         <v>110</v>
       </c>
-      <c r="D20" s="219" t="s">
-        <v>56</v>
-      </c>
-      <c r="E20" s="216" t="s">
+      <c r="D20" s="169" t="s">
+        <v>61</v>
+      </c>
+      <c r="E20" s="167" t="s">
         <v>313</v>
       </c>
-      <c r="F20" s="218" t="s">
+      <c r="F20" s="168" t="s">
         <v>111</v>
       </c>
       <c r="G20" s="81"/>
@@ -14184,19 +14229,19 @@
       <c r="A21" s="139" t="s">
         <v>56</v>
       </c>
-      <c r="B21" s="222" t="s">
+      <c r="B21" s="172" t="s">
         <v>283</v>
       </c>
-      <c r="C21" s="218" t="s">
+      <c r="C21" s="168" t="s">
         <v>112</v>
       </c>
-      <c r="D21" s="219" t="s">
+      <c r="D21" s="169" t="s">
         <v>56</v>
       </c>
-      <c r="E21" s="216" t="s">
+      <c r="E21" s="167" t="s">
         <v>314</v>
       </c>
-      <c r="F21" s="218" t="s">
+      <c r="F21" s="168" t="s">
         <v>113</v>
       </c>
       <c r="G21" s="81"/>
@@ -14255,21 +14300,21 @@
     </row>
     <row r="22" spans="1:59" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="139" t="s">
+        <v>61</v>
+      </c>
+      <c r="B22" s="172" t="s">
+        <v>284</v>
+      </c>
+      <c r="C22" s="168" t="s">
+        <v>114</v>
+      </c>
+      <c r="D22" s="169" t="s">
         <v>56</v>
       </c>
-      <c r="B22" s="222" t="s">
-        <v>284</v>
-      </c>
-      <c r="C22" s="218" t="s">
-        <v>114</v>
-      </c>
-      <c r="D22" s="219" t="s">
-        <v>56</v>
-      </c>
-      <c r="E22" s="216" t="s">
+      <c r="E22" s="167" t="s">
         <v>315</v>
       </c>
-      <c r="F22" s="218" t="s">
+      <c r="F22" s="168" t="s">
         <v>115</v>
       </c>
       <c r="G22" s="81"/>
@@ -14328,21 +14373,21 @@
     </row>
     <row r="23" spans="1:59" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="139" t="s">
-        <v>56</v>
-      </c>
-      <c r="B23" s="222" t="s">
+        <v>61</v>
+      </c>
+      <c r="B23" s="172" t="s">
         <v>285</v>
       </c>
-      <c r="C23" s="218" t="s">
+      <c r="C23" s="168" t="s">
         <v>116</v>
       </c>
-      <c r="D23" s="219" t="s">
-        <v>56</v>
-      </c>
-      <c r="E23" s="216" t="s">
+      <c r="D23" s="169" t="s">
+        <v>61</v>
+      </c>
+      <c r="E23" s="167" t="s">
         <v>316</v>
       </c>
-      <c r="F23" s="218" t="s">
+      <c r="F23" s="168" t="s">
         <v>117</v>
       </c>
       <c r="G23" s="81"/>
@@ -14401,21 +14446,21 @@
     </row>
     <row r="24" spans="1:59" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="139" t="s">
-        <v>56</v>
-      </c>
-      <c r="B24" s="222" t="s">
+        <v>61</v>
+      </c>
+      <c r="B24" s="172" t="s">
         <v>286</v>
       </c>
-      <c r="C24" s="218" t="s">
+      <c r="C24" s="168" t="s">
         <v>118</v>
       </c>
-      <c r="D24" s="219" t="s">
-        <v>56</v>
-      </c>
-      <c r="E24" s="216" t="s">
+      <c r="D24" s="169" t="s">
+        <v>61</v>
+      </c>
+      <c r="E24" s="167" t="s">
         <v>317</v>
       </c>
-      <c r="F24" s="218" t="s">
+      <c r="F24" s="168" t="s">
         <v>119</v>
       </c>
       <c r="G24" s="81"/>
@@ -14474,21 +14519,21 @@
     </row>
     <row r="25" spans="1:59" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="139" t="s">
-        <v>56</v>
-      </c>
-      <c r="B25" s="222" t="s">
+        <v>61</v>
+      </c>
+      <c r="B25" s="172" t="s">
         <v>287</v>
       </c>
-      <c r="C25" s="218" t="s">
+      <c r="C25" s="168" t="s">
         <v>120</v>
       </c>
-      <c r="D25" s="219" t="s">
-        <v>56</v>
-      </c>
-      <c r="E25" s="216" t="s">
+      <c r="D25" s="169" t="s">
+        <v>61</v>
+      </c>
+      <c r="E25" s="167" t="s">
         <v>318</v>
       </c>
-      <c r="F25" s="218" t="s">
+      <c r="F25" s="168" t="s">
         <v>121</v>
       </c>
       <c r="G25" s="81"/>
@@ -14547,21 +14592,21 @@
     </row>
     <row r="26" spans="1:59" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="139" t="s">
-        <v>56</v>
-      </c>
-      <c r="B26" s="222" t="s">
+        <v>61</v>
+      </c>
+      <c r="B26" s="172" t="s">
         <v>288</v>
       </c>
-      <c r="C26" s="218" t="s">
+      <c r="C26" s="168" t="s">
         <v>122</v>
       </c>
-      <c r="D26" s="219" t="s">
-        <v>56</v>
-      </c>
-      <c r="E26" s="216" t="s">
+      <c r="D26" s="169" t="s">
+        <v>61</v>
+      </c>
+      <c r="E26" s="167" t="s">
         <v>319</v>
       </c>
-      <c r="F26" s="218" t="s">
+      <c r="F26" s="168" t="s">
         <v>123</v>
       </c>
       <c r="G26" s="81"/>
@@ -14620,21 +14665,21 @@
     </row>
     <row r="27" spans="1:59" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="139" t="s">
-        <v>56</v>
-      </c>
-      <c r="B27" s="222" t="s">
+        <v>61</v>
+      </c>
+      <c r="B27" s="172" t="s">
         <v>289</v>
       </c>
-      <c r="C27" s="218" t="s">
+      <c r="C27" s="168" t="s">
         <v>124</v>
       </c>
-      <c r="D27" s="219" t="s">
-        <v>56</v>
-      </c>
-      <c r="E27" s="216" t="s">
+      <c r="D27" s="169" t="s">
+        <v>61</v>
+      </c>
+      <c r="E27" s="167" t="s">
         <v>320</v>
       </c>
-      <c r="F27" s="218" t="s">
+      <c r="F27" s="168" t="s">
         <v>125</v>
       </c>
       <c r="G27" s="81"/>
@@ -14695,19 +14740,19 @@
       <c r="A28" s="139" t="s">
         <v>61</v>
       </c>
-      <c r="B28" s="222" t="s">
+      <c r="B28" s="172" t="s">
         <v>290</v>
       </c>
-      <c r="C28" s="218" t="s">
+      <c r="C28" s="168" t="s">
         <v>126</v>
       </c>
-      <c r="D28" s="219" t="s">
-        <v>56</v>
-      </c>
-      <c r="E28" s="216" t="s">
+      <c r="D28" s="169" t="s">
+        <v>61</v>
+      </c>
+      <c r="E28" s="167" t="s">
         <v>321</v>
       </c>
-      <c r="F28" s="218" t="s">
+      <c r="F28" s="168" t="s">
         <v>127</v>
       </c>
       <c r="G28" s="81"/>
@@ -14766,21 +14811,21 @@
     </row>
     <row r="29" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A29" s="139" t="s">
-        <v>56</v>
-      </c>
-      <c r="B29" s="222" t="s">
+        <v>61</v>
+      </c>
+      <c r="B29" s="172" t="s">
         <v>291</v>
       </c>
-      <c r="C29" s="218" t="s">
+      <c r="C29" s="168" t="s">
         <v>128</v>
       </c>
-      <c r="D29" s="219" t="s">
-        <v>56</v>
-      </c>
-      <c r="E29" s="216" t="s">
+      <c r="D29" s="169" t="s">
+        <v>61</v>
+      </c>
+      <c r="E29" s="167" t="s">
         <v>322</v>
       </c>
-      <c r="F29" s="218" t="s">
+      <c r="F29" s="168" t="s">
         <v>129</v>
       </c>
       <c r="G29" s="81"/>
@@ -14839,21 +14884,21 @@
     </row>
     <row r="30" spans="1:59" s="81" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="139" t="s">
-        <v>56</v>
-      </c>
-      <c r="B30" s="222" t="s">
+        <v>61</v>
+      </c>
+      <c r="B30" s="172" t="s">
         <v>292</v>
       </c>
-      <c r="C30" s="218" t="s">
+      <c r="C30" s="168" t="s">
         <v>130</v>
       </c>
-      <c r="D30" s="220" t="s">
-        <v>56</v>
-      </c>
-      <c r="E30" s="216" t="s">
+      <c r="D30" s="170" t="s">
+        <v>61</v>
+      </c>
+      <c r="E30" s="167" t="s">
         <v>323</v>
       </c>
-      <c r="F30" s="218" t="s">
+      <c r="F30" s="168" t="s">
         <v>131</v>
       </c>
       <c r="I30" s="82"/>
@@ -14910,12 +14955,12 @@
     </row>
     <row r="31" spans="1:59" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="140" t="s">
-        <v>56</v>
-      </c>
-      <c r="B31" s="222" t="s">
+        <v>61</v>
+      </c>
+      <c r="B31" s="172" t="s">
         <v>293</v>
       </c>
-      <c r="C31" s="218" t="s">
+      <c r="C31" s="168" t="s">
         <v>132</v>
       </c>
       <c r="D31" s="81"/>
@@ -26745,10 +26790,10 @@
       <c r="AH1" s="65"/>
     </row>
     <row r="2" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="198" t="s">
+      <c r="A2" s="216" t="s">
         <v>143</v>
       </c>
-      <c r="B2" s="202">
+      <c r="B2" s="220">
         <v>1</v>
       </c>
       <c r="C2" s="69" t="s">
@@ -26804,8 +26849,8 @@
       <c r="AH2" s="66"/>
     </row>
     <row r="3" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A3" s="199"/>
-      <c r="B3" s="196"/>
+      <c r="A3" s="217"/>
+      <c r="B3" s="214"/>
       <c r="C3" s="71" t="s">
         <v>145</v>
       </c>
@@ -26856,8 +26901,8 @@
       <c r="AH3" s="66"/>
     </row>
     <row r="4" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A4" s="199"/>
-      <c r="B4" s="196"/>
+      <c r="A4" s="217"/>
+      <c r="B4" s="214"/>
       <c r="C4" s="71" t="s">
         <v>146</v>
       </c>
@@ -26908,8 +26953,8 @@
       <c r="AH4" s="66"/>
     </row>
     <row r="5" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="199"/>
-      <c r="B5" s="201"/>
+      <c r="A5" s="217"/>
+      <c r="B5" s="219"/>
       <c r="C5" s="71" t="s">
         <v>147</v>
       </c>
@@ -26960,8 +27005,8 @@
       <c r="AH5" s="66"/>
     </row>
     <row r="6" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A6" s="199"/>
-      <c r="B6" s="196">
+      <c r="A6" s="217"/>
+      <c r="B6" s="214">
         <v>2</v>
       </c>
       <c r="C6" s="71" t="s">
@@ -27016,8 +27061,8 @@
       <c r="AH6" s="66"/>
     </row>
     <row r="7" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A7" s="199"/>
-      <c r="B7" s="196"/>
+      <c r="A7" s="217"/>
+      <c r="B7" s="214"/>
       <c r="C7" s="71" t="s">
         <v>149</v>
       </c>
@@ -27068,8 +27113,8 @@
       <c r="AH7" s="66"/>
     </row>
     <row r="8" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="199"/>
-      <c r="B8" s="196"/>
+      <c r="A8" s="217"/>
+      <c r="B8" s="214"/>
       <c r="C8" s="71" t="s">
         <v>150</v>
       </c>
@@ -27119,8 +27164,8 @@
       <c r="AH8" s="66"/>
     </row>
     <row r="9" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A9" s="199"/>
-      <c r="B9" s="196"/>
+      <c r="A9" s="217"/>
+      <c r="B9" s="214"/>
       <c r="C9" s="71" t="s">
         <v>151</v>
       </c>
@@ -27175,8 +27220,8 @@
       <c r="AH9" s="66"/>
     </row>
     <row r="10" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A10" s="199"/>
-      <c r="B10" s="196">
+      <c r="A10" s="217"/>
+      <c r="B10" s="214">
         <v>3</v>
       </c>
       <c r="C10" s="71" t="s">
@@ -27234,8 +27279,8 @@
       <c r="AH10" s="66"/>
     </row>
     <row r="11" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A11" s="199"/>
-      <c r="B11" s="196"/>
+      <c r="A11" s="217"/>
+      <c r="B11" s="214"/>
       <c r="C11" s="71" t="s">
         <v>156</v>
       </c>
@@ -27290,8 +27335,8 @@
       <c r="AH11" s="66"/>
     </row>
     <row r="12" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A12" s="199"/>
-      <c r="B12" s="196"/>
+      <c r="A12" s="217"/>
+      <c r="B12" s="214"/>
       <c r="C12" s="71" t="s">
         <v>158</v>
       </c>
@@ -27349,8 +27394,8 @@
       <c r="AH12" s="66"/>
     </row>
     <row r="13" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A13" s="199"/>
-      <c r="B13" s="196"/>
+      <c r="A13" s="217"/>
+      <c r="B13" s="214"/>
       <c r="C13" s="71" t="s">
         <v>163</v>
       </c>
@@ -27416,8 +27461,8 @@
       <c r="AH13" s="66"/>
     </row>
     <row r="14" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A14" s="199"/>
-      <c r="B14" s="196">
+      <c r="A14" s="217"/>
+      <c r="B14" s="214">
         <v>4</v>
       </c>
       <c r="C14" s="71" t="s">
@@ -27484,8 +27529,8 @@
       <c r="AH14" s="66"/>
     </row>
     <row r="15" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A15" s="199"/>
-      <c r="B15" s="196"/>
+      <c r="A15" s="217"/>
+      <c r="B15" s="214"/>
       <c r="C15" s="71" t="s">
         <v>166</v>
       </c>
@@ -27548,8 +27593,8 @@
       <c r="AH15" s="66"/>
     </row>
     <row r="16" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A16" s="199"/>
-      <c r="B16" s="196"/>
+      <c r="A16" s="217"/>
+      <c r="B16" s="214"/>
       <c r="C16" s="71" t="s">
         <v>167</v>
       </c>
@@ -27612,8 +27657,8 @@
       <c r="AH16" s="66"/>
     </row>
     <row r="17" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A17" s="199"/>
-      <c r="B17" s="196"/>
+      <c r="A17" s="217"/>
+      <c r="B17" s="214"/>
       <c r="C17" s="71" t="s">
         <v>168</v>
       </c>
@@ -27676,8 +27721,8 @@
       <c r="AH17" s="66"/>
     </row>
     <row r="18" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A18" s="199"/>
-      <c r="B18" s="196">
+      <c r="A18" s="217"/>
+      <c r="B18" s="214">
         <v>5</v>
       </c>
       <c r="C18" s="71" t="s">
@@ -27744,8 +27789,8 @@
       <c r="AH18" s="66"/>
     </row>
     <row r="19" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A19" s="199"/>
-      <c r="B19" s="196"/>
+      <c r="A19" s="217"/>
+      <c r="B19" s="214"/>
       <c r="C19" s="71" t="s">
         <v>170</v>
       </c>
@@ -27809,8 +27854,8 @@
       <c r="AH19" s="66"/>
     </row>
     <row r="20" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A20" s="199"/>
-      <c r="B20" s="196"/>
+      <c r="A20" s="217"/>
+      <c r="B20" s="214"/>
       <c r="C20" s="71" t="s">
         <v>171</v>
       </c>
@@ -27873,8 +27918,8 @@
       <c r="AH20" s="66"/>
     </row>
     <row r="21" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A21" s="199"/>
-      <c r="B21" s="196"/>
+      <c r="A21" s="217"/>
+      <c r="B21" s="214"/>
       <c r="C21" s="71" t="s">
         <v>172</v>
       </c>
@@ -27937,8 +27982,8 @@
       <c r="AG21" s="80"/>
     </row>
     <row r="22" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A22" s="199"/>
-      <c r="B22" s="196">
+      <c r="A22" s="217"/>
+      <c r="B22" s="214">
         <v>6</v>
       </c>
       <c r="C22" s="71" t="s">
@@ -28004,8 +28049,8 @@
       <c r="AG22" s="80"/>
     </row>
     <row r="23" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A23" s="199"/>
-      <c r="B23" s="196"/>
+      <c r="A23" s="217"/>
+      <c r="B23" s="214"/>
       <c r="C23" s="71" t="s">
         <v>174</v>
       </c>
@@ -28070,8 +28115,8 @@
       <c r="AG23" s="80"/>
     </row>
     <row r="24" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A24" s="199"/>
-      <c r="B24" s="196"/>
+      <c r="A24" s="217"/>
+      <c r="B24" s="214"/>
       <c r="C24" s="71" t="s">
         <v>175</v>
       </c>
@@ -28132,8 +28177,8 @@
       <c r="AG24" s="80"/>
     </row>
     <row r="25" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A25" s="199"/>
-      <c r="B25" s="196"/>
+      <c r="A25" s="217"/>
+      <c r="B25" s="214"/>
       <c r="C25" s="71" t="s">
         <v>176</v>
       </c>
@@ -28191,8 +28236,8 @@
       <c r="AG25" s="66"/>
     </row>
     <row r="26" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A26" s="199"/>
-      <c r="B26" s="196">
+      <c r="A26" s="217"/>
+      <c r="B26" s="214">
         <v>7</v>
       </c>
       <c r="C26" s="71" t="s">
@@ -28252,8 +28297,8 @@
       <c r="AG26" s="66"/>
     </row>
     <row r="27" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A27" s="199"/>
-      <c r="B27" s="196"/>
+      <c r="A27" s="217"/>
+      <c r="B27" s="214"/>
       <c r="C27" s="71" t="s">
         <v>178</v>
       </c>
@@ -28309,8 +28354,8 @@
       </c>
     </row>
     <row r="28" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A28" s="199"/>
-      <c r="B28" s="196"/>
+      <c r="A28" s="217"/>
+      <c r="B28" s="214"/>
       <c r="C28" s="71" t="s">
         <v>180</v>
       </c>
@@ -28366,8 +28411,8 @@
       </c>
     </row>
     <row r="29" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A29" s="199"/>
-      <c r="B29" s="196"/>
+      <c r="A29" s="217"/>
+      <c r="B29" s="214"/>
       <c r="C29" s="71" t="s">
         <v>182</v>
       </c>
@@ -28424,8 +28469,8 @@
       </c>
     </row>
     <row r="30" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A30" s="199"/>
-      <c r="B30" s="196">
+      <c r="A30" s="217"/>
+      <c r="B30" s="214">
         <v>8</v>
       </c>
       <c r="C30" s="71" t="s">
@@ -28483,8 +28528,8 @@
       </c>
     </row>
     <row r="31" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A31" s="199"/>
-      <c r="B31" s="196"/>
+      <c r="A31" s="217"/>
+      <c r="B31" s="214"/>
       <c r="C31" s="71" t="s">
         <v>187</v>
       </c>
@@ -28539,8 +28584,8 @@
       </c>
     </row>
     <row r="32" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A32" s="199"/>
-      <c r="B32" s="196"/>
+      <c r="A32" s="217"/>
+      <c r="B32" s="214"/>
       <c r="C32" s="71" t="s">
         <v>189</v>
       </c>
@@ -28590,8 +28635,8 @@
       </c>
     </row>
     <row r="33" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A33" s="199"/>
-      <c r="B33" s="196"/>
+      <c r="A33" s="217"/>
+      <c r="B33" s="214"/>
       <c r="C33" s="71" t="s">
         <v>190</v>
       </c>
@@ -28637,8 +28682,8 @@
       <c r="AA33" s="66"/>
     </row>
     <row r="34" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A34" s="199"/>
-      <c r="B34" s="196">
+      <c r="A34" s="217"/>
+      <c r="B34" s="214">
         <v>9</v>
       </c>
       <c r="C34" s="71" t="s">
@@ -28684,8 +28729,8 @@
       <c r="AA34" s="66"/>
     </row>
     <row r="35" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A35" s="199"/>
-      <c r="B35" s="196"/>
+      <c r="A35" s="217"/>
+      <c r="B35" s="214"/>
       <c r="C35" s="71" t="s">
         <v>192</v>
       </c>
@@ -28728,8 +28773,8 @@
       <c r="AA35" s="66"/>
     </row>
     <row r="36" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A36" s="199"/>
-      <c r="B36" s="196"/>
+      <c r="A36" s="217"/>
+      <c r="B36" s="214"/>
       <c r="C36" s="71" t="s">
         <v>193</v>
       </c>
@@ -28774,8 +28819,8 @@
       <c r="AA36" s="66"/>
     </row>
     <row r="37" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A37" s="199"/>
-      <c r="B37" s="196"/>
+      <c r="A37" s="217"/>
+      <c r="B37" s="214"/>
       <c r="C37" s="71" t="s">
         <v>194</v>
       </c>
@@ -28818,8 +28863,8 @@
       <c r="AA37" s="66"/>
     </row>
     <row r="38" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A38" s="199"/>
-      <c r="B38" s="196">
+      <c r="A38" s="217"/>
+      <c r="B38" s="214">
         <v>10</v>
       </c>
       <c r="C38" s="71" t="s">
@@ -28867,8 +28912,8 @@
       <c r="AH38" s="66"/>
     </row>
     <row r="39" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A39" s="199"/>
-      <c r="B39" s="196"/>
+      <c r="A39" s="217"/>
+      <c r="B39" s="214"/>
       <c r="C39" s="71" t="s">
         <v>196</v>
       </c>
@@ -28913,8 +28958,8 @@
       <c r="AH39" s="66"/>
     </row>
     <row r="40" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A40" s="199"/>
-      <c r="B40" s="196"/>
+      <c r="A40" s="217"/>
+      <c r="B40" s="214"/>
       <c r="C40" s="71" t="s">
         <v>197</v>
       </c>
@@ -28958,8 +29003,8 @@
       <c r="AH40" s="66"/>
     </row>
     <row r="41" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A41" s="199"/>
-      <c r="B41" s="196"/>
+      <c r="A41" s="217"/>
+      <c r="B41" s="214"/>
       <c r="C41" s="71" t="s">
         <v>198</v>
       </c>
@@ -29009,8 +29054,8 @@
       <c r="AH41" s="66"/>
     </row>
     <row r="42" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A42" s="199"/>
-      <c r="B42" s="196">
+      <c r="A42" s="217"/>
+      <c r="B42" s="214">
         <v>11</v>
       </c>
       <c r="C42" s="71" t="s">
@@ -29063,8 +29108,8 @@
       <c r="AH42" s="66"/>
     </row>
     <row r="43" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A43" s="199"/>
-      <c r="B43" s="196"/>
+      <c r="A43" s="217"/>
+      <c r="B43" s="214"/>
       <c r="C43" s="71" t="s">
         <v>200</v>
       </c>
@@ -29117,8 +29162,8 @@
       <c r="AH43" s="66"/>
     </row>
     <row r="44" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A44" s="199"/>
-      <c r="B44" s="196"/>
+      <c r="A44" s="217"/>
+      <c r="B44" s="214"/>
       <c r="C44" s="71" t="s">
         <v>201</v>
       </c>
@@ -29168,8 +29213,8 @@
       <c r="AH44" s="66"/>
     </row>
     <row r="45" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A45" s="199"/>
-      <c r="B45" s="196"/>
+      <c r="A45" s="217"/>
+      <c r="B45" s="214"/>
       <c r="C45" s="71" t="s">
         <v>202</v>
       </c>
@@ -29219,8 +29264,8 @@
       <c r="AH45" s="66"/>
     </row>
     <row r="46" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A46" s="199"/>
-      <c r="B46" s="196">
+      <c r="A46" s="217"/>
+      <c r="B46" s="214">
         <v>12</v>
       </c>
       <c r="C46" s="71" t="s">
@@ -29274,8 +29319,8 @@
       <c r="AH46" s="66"/>
     </row>
     <row r="47" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A47" s="199"/>
-      <c r="B47" s="196"/>
+      <c r="A47" s="217"/>
+      <c r="B47" s="214"/>
       <c r="C47" s="71" t="s">
         <v>204</v>
       </c>
@@ -29325,8 +29370,8 @@
       <c r="AH47" s="66"/>
     </row>
     <row r="48" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A48" s="199"/>
-      <c r="B48" s="196"/>
+      <c r="A48" s="217"/>
+      <c r="B48" s="214"/>
       <c r="C48" s="71" t="s">
         <v>205</v>
       </c>
@@ -29378,8 +29423,8 @@
       <c r="AH48" s="66"/>
     </row>
     <row r="49" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A49" s="199"/>
-      <c r="B49" s="196"/>
+      <c r="A49" s="217"/>
+      <c r="B49" s="214"/>
       <c r="C49" s="71" t="s">
         <v>206</v>
       </c>
@@ -29429,8 +29474,8 @@
       <c r="AH49" s="66"/>
     </row>
     <row r="50" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A50" s="199"/>
-      <c r="B50" s="196">
+      <c r="A50" s="217"/>
+      <c r="B50" s="214">
         <v>13</v>
       </c>
       <c r="C50" s="71" t="s">
@@ -29484,8 +29529,8 @@
       <c r="AH50" s="66"/>
     </row>
     <row r="51" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A51" s="199"/>
-      <c r="B51" s="196"/>
+      <c r="A51" s="217"/>
+      <c r="B51" s="214"/>
       <c r="C51" s="71" t="s">
         <v>208</v>
       </c>
@@ -29535,8 +29580,8 @@
       <c r="AH51" s="66"/>
     </row>
     <row r="52" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A52" s="199"/>
-      <c r="B52" s="196"/>
+      <c r="A52" s="217"/>
+      <c r="B52" s="214"/>
       <c r="C52" s="71" t="s">
         <v>209</v>
       </c>
@@ -29585,8 +29630,8 @@
       <c r="AH52" s="66"/>
     </row>
     <row r="53" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A53" s="199"/>
-      <c r="B53" s="196"/>
+      <c r="A53" s="217"/>
+      <c r="B53" s="214"/>
       <c r="C53" s="71" t="s">
         <v>210</v>
       </c>
@@ -29636,8 +29681,8 @@
       <c r="AH53" s="66"/>
     </row>
     <row r="54" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="199"/>
-      <c r="B54" s="196">
+      <c r="A54" s="217"/>
+      <c r="B54" s="214">
         <v>14</v>
       </c>
       <c r="C54" s="71" t="s">
@@ -29691,8 +29736,8 @@
       <c r="AH54" s="66"/>
     </row>
     <row r="55" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A55" s="199"/>
-      <c r="B55" s="196"/>
+      <c r="A55" s="217"/>
+      <c r="B55" s="214"/>
       <c r="C55" s="71" t="s">
         <v>212</v>
       </c>
@@ -29743,8 +29788,8 @@
       <c r="AH55" s="66"/>
     </row>
     <row r="56" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A56" s="199"/>
-      <c r="B56" s="196"/>
+      <c r="A56" s="217"/>
+      <c r="B56" s="214"/>
       <c r="C56" s="71" t="s">
         <v>213</v>
       </c>
@@ -29794,8 +29839,8 @@
       <c r="AH56" s="66"/>
     </row>
     <row r="57" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A57" s="199"/>
-      <c r="B57" s="196"/>
+      <c r="A57" s="217"/>
+      <c r="B57" s="214"/>
       <c r="C57" s="71" t="s">
         <v>214</v>
       </c>
@@ -29846,8 +29891,8 @@
       <c r="AH57" s="66"/>
     </row>
     <row r="58" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A58" s="199"/>
-      <c r="B58" s="196">
+      <c r="A58" s="217"/>
+      <c r="B58" s="214">
         <v>15</v>
       </c>
       <c r="C58" s="71" t="s">
@@ -29902,8 +29947,8 @@
       <c r="AH58" s="66"/>
     </row>
     <row r="59" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A59" s="199"/>
-      <c r="B59" s="196"/>
+      <c r="A59" s="217"/>
+      <c r="B59" s="214"/>
       <c r="C59" s="71" t="s">
         <v>216</v>
       </c>
@@ -29954,8 +29999,8 @@
       <c r="AH59" s="66"/>
     </row>
     <row r="60" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A60" s="199"/>
-      <c r="B60" s="196"/>
+      <c r="A60" s="217"/>
+      <c r="B60" s="214"/>
       <c r="C60" s="71" t="s">
         <v>217</v>
       </c>
@@ -30006,8 +30051,8 @@
       <c r="AH60" s="66"/>
     </row>
     <row r="61" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A61" s="200"/>
-      <c r="B61" s="197"/>
+      <c r="A61" s="218"/>
+      <c r="B61" s="215"/>
       <c r="C61" s="73" t="s">
         <v>218</v>
       </c>
@@ -30058,10 +30103,10 @@
       <c r="AH61" s="66"/>
     </row>
     <row r="62" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A62" s="198" t="s">
+      <c r="A62" s="216" t="s">
         <v>137</v>
       </c>
-      <c r="B62" s="201">
+      <c r="B62" s="219">
         <v>16</v>
       </c>
       <c r="C62" s="71" t="s">
@@ -30099,7 +30144,7 @@
         <v>0</v>
       </c>
       <c r="Y62" s="72">
-        <f t="shared" ref="Y62:Y65" si="5">SUM(U62:X62)</f>
+        <f>SUM(U62:X62)</f>
         <v>0</v>
       </c>
       <c r="Z62" s="66"/>
@@ -30113,8 +30158,8 @@
       <c r="AH62" s="66"/>
     </row>
     <row r="63" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A63" s="199"/>
-      <c r="B63" s="196"/>
+      <c r="A63" s="217"/>
+      <c r="B63" s="214"/>
       <c r="C63" s="71" t="s">
         <v>220</v>
       </c>
@@ -30150,7 +30195,7 @@
         <v>0</v>
       </c>
       <c r="Y63" s="72">
-        <f t="shared" si="5"/>
+        <f>SUM(U63:X63)</f>
         <v>0</v>
       </c>
       <c r="Z63" s="66"/>
@@ -30164,8 +30209,8 @@
       <c r="AH63" s="66"/>
     </row>
     <row r="64" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A64" s="199"/>
-      <c r="B64" s="196"/>
+      <c r="A64" s="217"/>
+      <c r="B64" s="214"/>
       <c r="C64" s="71" t="s">
         <v>221</v>
       </c>
@@ -30201,7 +30246,7 @@
         <v>0</v>
       </c>
       <c r="Y64" s="72">
-        <f t="shared" si="5"/>
+        <f>SUM(U64:X64)</f>
         <v>0</v>
       </c>
       <c r="Z64" s="66"/>
@@ -30215,8 +30260,8 @@
       <c r="AH64" s="66"/>
     </row>
     <row r="65" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A65" s="199"/>
-      <c r="B65" s="196"/>
+      <c r="A65" s="217"/>
+      <c r="B65" s="214"/>
       <c r="C65" s="71" t="s">
         <v>222</v>
       </c>
@@ -30252,7 +30297,7 @@
         <v>0</v>
       </c>
       <c r="Y65" s="72">
-        <f t="shared" si="5"/>
+        <f>SUM(U65:X65)</f>
         <v>0</v>
       </c>
       <c r="Z65" s="66"/>
@@ -30266,8 +30311,8 @@
       <c r="AH65" s="66"/>
     </row>
     <row r="66" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A66" s="199"/>
-      <c r="B66" s="196">
+      <c r="A66" s="217"/>
+      <c r="B66" s="214">
         <v>17</v>
       </c>
       <c r="C66" s="71" t="s">
@@ -30305,7 +30350,7 @@
         <v>0</v>
       </c>
       <c r="Y66" s="72">
-        <f t="shared" ref="Y66:Y77" si="6">SUM(U66:X66)</f>
+        <f t="shared" ref="Y66:Y77" si="5">SUM(U66:X66)</f>
         <v>0</v>
       </c>
       <c r="Z66" s="66"/>
@@ -30319,8 +30364,8 @@
       <c r="AH66" s="66"/>
     </row>
     <row r="67" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A67" s="199"/>
-      <c r="B67" s="196"/>
+      <c r="A67" s="217"/>
+      <c r="B67" s="214"/>
       <c r="C67" s="71" t="s">
         <v>224</v>
       </c>
@@ -30356,7 +30401,7 @@
         <v>0</v>
       </c>
       <c r="Y67" s="72">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="Z67" s="66"/>
@@ -30370,8 +30415,8 @@
       <c r="AH67" s="66"/>
     </row>
     <row r="68" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A68" s="199"/>
-      <c r="B68" s="196"/>
+      <c r="A68" s="217"/>
+      <c r="B68" s="214"/>
       <c r="C68" s="71" t="s">
         <v>225</v>
       </c>
@@ -30407,7 +30452,7 @@
         <v>0</v>
       </c>
       <c r="Y68" s="72">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="Z68" s="66"/>
@@ -30421,8 +30466,8 @@
       <c r="AH68" s="66"/>
     </row>
     <row r="69" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A69" s="199"/>
-      <c r="B69" s="196"/>
+      <c r="A69" s="217"/>
+      <c r="B69" s="214"/>
       <c r="C69" s="71" t="s">
         <v>226</v>
       </c>
@@ -30458,7 +30503,7 @@
         <v>0</v>
       </c>
       <c r="Y69" s="72">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="Z69" s="66"/>
@@ -30472,8 +30517,8 @@
       <c r="AH69" s="66"/>
     </row>
     <row r="70" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A70" s="199"/>
-      <c r="B70" s="196">
+      <c r="A70" s="217"/>
+      <c r="B70" s="214">
         <v>18</v>
       </c>
       <c r="C70" s="71" t="s">
@@ -30511,7 +30556,7 @@
         <v>0</v>
       </c>
       <c r="Y70" s="72">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="Z70" s="66"/>
@@ -30525,8 +30570,8 @@
       <c r="AH70" s="66"/>
     </row>
     <row r="71" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A71" s="199"/>
-      <c r="B71" s="196"/>
+      <c r="A71" s="217"/>
+      <c r="B71" s="214"/>
       <c r="C71" s="71" t="s">
         <v>228</v>
       </c>
@@ -30562,7 +30607,7 @@
         <v>0</v>
       </c>
       <c r="Y71" s="72">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="Z71" s="66"/>
@@ -30576,8 +30621,8 @@
       <c r="AH71" s="66"/>
     </row>
     <row r="72" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A72" s="199"/>
-      <c r="B72" s="196"/>
+      <c r="A72" s="217"/>
+      <c r="B72" s="214"/>
       <c r="C72" s="71" t="s">
         <v>229</v>
       </c>
@@ -30613,7 +30658,7 @@
         <v>0</v>
       </c>
       <c r="Y72" s="72">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="Z72" s="66"/>
@@ -30627,8 +30672,8 @@
       <c r="AH72" s="66"/>
     </row>
     <row r="73" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A73" s="199"/>
-      <c r="B73" s="196"/>
+      <c r="A73" s="217"/>
+      <c r="B73" s="214"/>
       <c r="C73" s="71" t="s">
         <v>230</v>
       </c>
@@ -30664,7 +30709,7 @@
         <v>0</v>
       </c>
       <c r="Y73" s="72">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="Z73" s="66"/>
@@ -30678,8 +30723,8 @@
       <c r="AH73" s="66"/>
     </row>
     <row r="74" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A74" s="199"/>
-      <c r="B74" s="196">
+      <c r="A74" s="217"/>
+      <c r="B74" s="214">
         <v>19</v>
       </c>
       <c r="C74" s="71" t="s">
@@ -30717,7 +30762,7 @@
         <v>0</v>
       </c>
       <c r="Y74" s="72">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="Z74" s="66"/>
@@ -30731,8 +30776,8 @@
       <c r="AH74" s="66"/>
     </row>
     <row r="75" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A75" s="199"/>
-      <c r="B75" s="196"/>
+      <c r="A75" s="217"/>
+      <c r="B75" s="214"/>
       <c r="C75" s="71" t="s">
         <v>232</v>
       </c>
@@ -30768,7 +30813,7 @@
         <v>0</v>
       </c>
       <c r="Y75" s="72">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="Z75" s="66"/>
@@ -30782,8 +30827,8 @@
       <c r="AH75" s="66"/>
     </row>
     <row r="76" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A76" s="199"/>
-      <c r="B76" s="196"/>
+      <c r="A76" s="217"/>
+      <c r="B76" s="214"/>
       <c r="C76" s="71" t="s">
         <v>233</v>
       </c>
@@ -30819,7 +30864,7 @@
         <v>0</v>
       </c>
       <c r="Y76" s="72">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="Z76" s="66"/>
@@ -30833,8 +30878,8 @@
       <c r="AH76" s="66"/>
     </row>
     <row r="77" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A77" s="200"/>
-      <c r="B77" s="197"/>
+      <c r="A77" s="218"/>
+      <c r="B77" s="215"/>
       <c r="C77" s="73" t="s">
         <v>234</v>
       </c>
@@ -30870,7 +30915,7 @@
         <v>0</v>
       </c>
       <c r="Y77" s="74">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="Z77" s="66"/>
@@ -30892,63 +30937,63 @@
         <v>0</v>
       </c>
       <c r="E78" s="87">
-        <f t="shared" ref="E78:S78" si="7">SUM(E2:E77)</f>
+        <f t="shared" ref="E78:S78" si="6">SUM(E2:E77)</f>
         <v>4</v>
       </c>
       <c r="F78" s="87">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>12</v>
       </c>
       <c r="G78" s="87">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>15</v>
       </c>
       <c r="H78" s="87">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>27</v>
       </c>
       <c r="I78" s="87">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>12</v>
       </c>
       <c r="J78" s="87">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>24</v>
       </c>
       <c r="K78" s="87">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>9</v>
       </c>
       <c r="L78" s="87">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>12</v>
       </c>
       <c r="M78" s="87">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>21</v>
       </c>
       <c r="N78" s="87">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>18</v>
       </c>
       <c r="O78" s="87">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>15</v>
       </c>
       <c r="P78" s="87">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>15</v>
       </c>
       <c r="Q78" s="87">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>9</v>
       </c>
       <c r="R78" s="87">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>30</v>
       </c>
       <c r="S78" s="87">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="T78" s="66"/>
@@ -31021,10 +31066,10 @@
     <row r="80" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A80" s="66"/>
       <c r="B80" s="66"/>
-      <c r="C80" s="205" t="s">
+      <c r="C80" s="210" t="s">
         <v>235</v>
       </c>
-      <c r="D80" s="206"/>
+      <c r="D80" s="211"/>
       <c r="E80" s="70">
         <v>60</v>
       </c>
@@ -31063,10 +31108,10 @@
     <row r="81" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A81" s="66"/>
       <c r="B81" s="66"/>
-      <c r="C81" s="207" t="s">
+      <c r="C81" s="212" t="s">
         <v>237</v>
       </c>
-      <c r="D81" s="208"/>
+      <c r="D81" s="213"/>
       <c r="E81" s="72">
         <v>322.5</v>
       </c>
@@ -31103,10 +31148,10 @@
     <row r="82" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A82" s="66"/>
       <c r="B82" s="66"/>
-      <c r="C82" s="207" t="s">
+      <c r="C82" s="212" t="s">
         <v>238</v>
       </c>
-      <c r="D82" s="208"/>
+      <c r="D82" s="213"/>
       <c r="E82" s="72">
         <v>35</v>
       </c>
@@ -31143,10 +31188,10 @@
     <row r="83" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A83" s="66"/>
       <c r="B83" s="66"/>
-      <c r="C83" s="207" t="s">
+      <c r="C83" s="212" t="s">
         <v>239</v>
       </c>
-      <c r="D83" s="208"/>
+      <c r="D83" s="213"/>
       <c r="E83" s="72">
         <v>287</v>
       </c>
@@ -31183,10 +31228,10 @@
     <row r="84" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A84" s="66"/>
       <c r="B84" s="66"/>
-      <c r="C84" s="207" t="s">
+      <c r="C84" s="212" t="s">
         <v>240</v>
       </c>
-      <c r="D84" s="208"/>
+      <c r="D84" s="213"/>
       <c r="E84" s="72">
         <v>60</v>
       </c>
@@ -31223,10 +31268,10 @@
     <row r="85" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A85" s="66"/>
       <c r="B85" s="66"/>
-      <c r="C85" s="203" t="s">
+      <c r="C85" s="208" t="s">
         <v>241</v>
       </c>
-      <c r="D85" s="204"/>
+      <c r="D85" s="209"/>
       <c r="E85" s="74">
         <f>Y79</f>
         <v>483</v>
@@ -31294,17 +31339,6 @@
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="C85:D85"/>
-    <mergeCell ref="C80:D80"/>
-    <mergeCell ref="C81:D81"/>
-    <mergeCell ref="C82:D82"/>
-    <mergeCell ref="C83:D83"/>
-    <mergeCell ref="C84:D84"/>
-    <mergeCell ref="B22:B25"/>
-    <mergeCell ref="B26:B29"/>
-    <mergeCell ref="B30:B33"/>
-    <mergeCell ref="B34:B37"/>
-    <mergeCell ref="B38:B41"/>
     <mergeCell ref="B66:B69"/>
     <mergeCell ref="B70:B73"/>
     <mergeCell ref="B74:B77"/>
@@ -31321,6 +31355,17 @@
     <mergeCell ref="B42:B45"/>
     <mergeCell ref="B46:B49"/>
     <mergeCell ref="B50:B53"/>
+    <mergeCell ref="B22:B25"/>
+    <mergeCell ref="B26:B29"/>
+    <mergeCell ref="B30:B33"/>
+    <mergeCell ref="B34:B37"/>
+    <mergeCell ref="B38:B41"/>
+    <mergeCell ref="C85:D85"/>
+    <mergeCell ref="C80:D80"/>
+    <mergeCell ref="C81:D81"/>
+    <mergeCell ref="C82:D82"/>
+    <mergeCell ref="C83:D83"/>
+    <mergeCell ref="C84:D84"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -31337,70 +31382,71 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="28" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="160" t="s">
+      <c r="A1" s="159" t="s">
         <v>331</v>
       </c>
-      <c r="B1" s="161" t="s">
+      <c r="B1" s="160" t="s">
         <v>341</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="160" t="s">
+      <c r="A2" s="159" t="s">
         <v>332</v>
       </c>
-      <c r="B2" s="162">
+      <c r="B2" s="161">
         <v>45579</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="160" t="s">
+      <c r="A3" s="159" t="s">
         <v>333</v>
       </c>
-      <c r="B3" s="163" t="s">
+      <c r="B3" s="162" t="s">
         <v>334</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="160" t="s">
+      <c r="A4" s="159" t="s">
         <v>335</v>
       </c>
-      <c r="B4" s="164" t="s">
+      <c r="B4" s="163" t="s">
         <v>336</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="160" t="s">
+      <c r="A5" s="159" t="s">
         <v>337</v>
       </c>
-      <c r="B5" s="165">
-        <v>1.2</v>
+      <c r="B5" s="164">
+        <v>1.3</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="160" t="s">
+      <c r="A6" s="159" t="s">
         <v>338</v>
       </c>
-      <c r="B6" s="162">
-        <v>45602</v>
+      <c r="B6" s="161">
+        <v>45632</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="160" t="s">
+      <c r="A7" s="159" t="s">
         <v>339</v>
       </c>
-      <c r="B7" s="163" t="s">
-        <v>347</v>
+      <c r="B7" s="162" t="s">
+        <v>356</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="160" t="s">
+      <c r="A8" s="159" t="s">
         <v>340</v>
       </c>
-      <c r="B8" s="161" t="s">
+      <c r="B8" s="160" t="s">
         <v>342</v>
       </c>
     </row>
@@ -31649,21 +31695,21 @@
     </row>
     <row r="5" spans="1:19" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
-      <c r="B5" s="209" t="s">
+      <c r="B5" s="221" t="s">
         <v>259</v>
       </c>
-      <c r="C5" s="210"/>
-      <c r="D5" s="210"/>
-      <c r="E5" s="210"/>
-      <c r="F5" s="210"/>
-      <c r="G5" s="210"/>
-      <c r="H5" s="210"/>
-      <c r="I5" s="210"/>
-      <c r="J5" s="210"/>
-      <c r="K5" s="210"/>
-      <c r="L5" s="210"/>
-      <c r="M5" s="210"/>
-      <c r="N5" s="211"/>
+      <c r="C5" s="222"/>
+      <c r="D5" s="222"/>
+      <c r="E5" s="222"/>
+      <c r="F5" s="222"/>
+      <c r="G5" s="222"/>
+      <c r="H5" s="222"/>
+      <c r="I5" s="222"/>
+      <c r="J5" s="222"/>
+      <c r="K5" s="222"/>
+      <c r="L5" s="222"/>
+      <c r="M5" s="222"/>
+      <c r="N5" s="223"/>
       <c r="O5" s="5"/>
       <c r="P5" s="2"/>
       <c r="Q5" s="2"/>
@@ -31743,21 +31789,21 @@
       <c r="F9" s="16"/>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B10" s="212" t="s">
+      <c r="B10" s="224" t="s">
         <v>261</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B11" s="212"/>
+      <c r="B11" s="224"/>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B12" s="212"/>
+      <c r="B12" s="224"/>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B13" s="212"/>
+      <c r="B13" s="224"/>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B14" s="212"/>
+      <c r="B14" s="224"/>
     </row>
     <row r="21" spans="18:18" x14ac:dyDescent="0.25">
       <c r="R21" s="18"/>
@@ -31777,37 +31823,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <SharedWithUsers xmlns="d03ffd70-462c-4172-9015-a0cdff42c83c">
-      <UserInfo>
-        <DisplayName>Craig Stevens</DisplayName>
-        <AccountId>17</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Afzan Matloob</DisplayName>
-        <AccountId>46</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="65f98c99-c090-489b-8346-b847c18a5011">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010060D9039996957B47A2820CA7E129C20F" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="61c230ac488284aa1c9442a337ce5a7f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="65f98c99-c090-489b-8346-b847c18a5011" xmlns:ns3="d03ffd70-462c-4172-9015-a0cdff42c83c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4cea2a2cd68f11dd2b0a1fdf049f3860" ns2:_="" ns3:_="">
     <xsd:import namespace="65f98c99-c090-489b-8346-b847c18a5011"/>
@@ -32024,10 +32039,52 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <SharedWithUsers xmlns="d03ffd70-462c-4172-9015-a0cdff42c83c">
+      <UserInfo>
+        <DisplayName>Craig Stevens</DisplayName>
+        <AccountId>17</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Afzan Matloob</DisplayName>
+        <AccountId>46</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="65f98c99-c090-489b-8346-b847c18a5011">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F7D0D882-CBE1-41A5-A59C-C48B26872275}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{710DD5DA-09F7-4D7C-A10A-C80CDC0D2E16}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="65f98c99-c090-489b-8346-b847c18a5011"/>
+    <ds:schemaRef ds:uri="d03ffd70-462c-4172-9015-a0cdff42c83c"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -32044,20 +32101,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{710DD5DA-09F7-4D7C-A10A-C80CDC0D2E16}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F7D0D882-CBE1-41A5-A59C-C48B26872275}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="65f98c99-c090-489b-8346-b847c18a5011"/>
-    <ds:schemaRef ds:uri="d03ffd70-462c-4172-9015-a0cdff42c83c"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>